<commit_message>
Update Checklist & Game Logic
Now Unitychan has 'HP', and is able to 'die'.
Problems on map status recording solved quite swimmingly.
Bad news, some work delayed due to other homework.
FA♂Q other homework.
Good news, L.M cleared E6 yesterday, with only ONE try.
</commit_message>
<xml_diff>
--- a/Docs/UniBOOM_Checklist.xlsx
+++ b/Docs/UniBOOM_Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="73">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -90,10 +90,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>简单Gameover逻辑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Unitychan受伤与倒地动画逻辑</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -126,18 +122,10 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>熟悉CSV读写</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>L.M</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>地图数据结构设计</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>整理代码</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -276,9 +264,6 @@
   <si>
     <t>修改地图要素记录逻辑</t>
     <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>简单开幕逻辑</t>
   </si>
   <si>
     <r>
@@ -299,12 +284,87 @@
     </r>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
+  <si>
+    <t>EnemyDummy.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unitychan.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Unitychan.controller</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Room.cs</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单Gameover逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地图数据结构设计</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>简单开幕逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Debug模式虽然加了不过目前没什么实际内容。
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>虽然昨天说是“大幅度修改”，结果改起来还挺方便的。这个没拖。</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="宋体"/>
+        <family val="2"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+简单Gameover逻辑、地图数据结构设计、简单开幕逻辑由于有其他作业，拖延至明天。
+熟悉CSV读写由于有其他作业，拖延至明天。
+其他作业FA♂Q。</t>
+    </r>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>熟悉CSV读写</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>熟悉CSV读写</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -323,6 +383,21 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="宋体"/>
       <family val="3"/>
       <charset val="134"/>
@@ -452,7 +527,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -462,24 +537,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -489,20 +573,23 @@
     <xf numFmtId="58" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -805,21 +892,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E53"/>
+  <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:E12"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A27" sqref="A27:E27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="2" max="2" width="12.25" customWidth="1"/>
     <col min="3" max="3" width="33" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.75" customWidth="1"/>
-    <col min="5" max="5" width="14" customWidth="1"/>
+    <col min="5" max="5" width="21.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="1" spans="1:5">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -836,7 +923,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:5">
       <c r="A2" s="7">
         <v>42128</v>
       </c>
@@ -846,57 +933,65 @@
       <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D2" s="4"/>
+      <c r="E2" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
       <c r="A3" s="7"/>
       <c r="B3" s="6"/>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D3" s="4"/>
+      <c r="E3" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
       <c r="A4" s="7"/>
       <c r="B4" s="6"/>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D4" s="4"/>
+      <c r="E4" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
       <c r="A5" s="7"/>
       <c r="B5" s="6"/>
       <c r="C5" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="13"/>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.15">
+        <v>18</v>
+      </c>
+      <c r="D5" s="5"/>
+      <c r="E5" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
       <c r="A6" s="7"/>
       <c r="B6" s="6"/>
       <c r="C6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D6" s="13"/>
+        <v>19</v>
+      </c>
+      <c r="D6" s="4"/>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="7" spans="1:5">
       <c r="A7" s="7"/>
       <c r="B7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="13"/>
+        <v>22</v>
+      </c>
+      <c r="D7" s="4"/>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="8" spans="1:5">
       <c r="A8" s="7"/>
       <c r="B8" s="2" t="s">
         <v>10</v>
@@ -904,10 +999,10 @@
       <c r="C8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="12"/>
+      <c r="D8" s="4"/>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="9" spans="1:5">
       <c r="A9" s="7"/>
       <c r="B9" s="6" t="s">
         <v>12</v>
@@ -915,37 +1010,37 @@
       <c r="C9" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D9" s="12"/>
+      <c r="D9" s="4"/>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="10" spans="1:5">
       <c r="A10" s="7"/>
       <c r="B10" s="6"/>
       <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D10" s="12"/>
+      <c r="D10" s="4"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="11" spans="1:5">
       <c r="A11" s="7"/>
       <c r="B11" s="6"/>
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="12"/>
+      <c r="D11" s="4"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" ht="49.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16"/>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="12" spans="1:5" ht="49.5" customHeight="1">
+      <c r="A12" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10"/>
+    </row>
+    <row r="13" spans="1:5">
       <c r="A13" s="7">
         <v>42129</v>
       </c>
@@ -955,407 +1050,471 @@
       <c r="C13" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="1"/>
+      <c r="D13" s="4"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="14" spans="1:5">
       <c r="A14" s="7"/>
       <c r="B14" s="6"/>
       <c r="C14" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.15">
+        <v>61</v>
+      </c>
+      <c r="D14" s="4"/>
+      <c r="E14" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
       <c r="A15" s="7"/>
       <c r="B15" s="6"/>
       <c r="C15" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.15">
+        <v>25</v>
+      </c>
+      <c r="D15" s="4"/>
+      <c r="E15" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
       <c r="A16" s="7"/>
       <c r="B16" s="6"/>
       <c r="C16" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.15">
+      <c r="D16" s="4"/>
+      <c r="E16" s="1" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
       <c r="A17" s="7"/>
       <c r="B17" s="6"/>
       <c r="C17" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D17" s="1"/>
+        <v>67</v>
+      </c>
+      <c r="D17" s="5"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="18" spans="1:5">
       <c r="A18" s="7"/>
       <c r="B18" s="6"/>
       <c r="C18" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D18" s="1"/>
+        <v>68</v>
+      </c>
+      <c r="D18" s="5"/>
       <c r="E18" s="1"/>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="19" spans="1:5">
       <c r="A19" s="7"/>
       <c r="B19" s="6"/>
       <c r="C19" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="D19" s="1"/>
+        <v>69</v>
+      </c>
+      <c r="D19" s="5"/>
       <c r="E19" s="1"/>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="20" spans="1:5">
       <c r="A20" s="7"/>
       <c r="B20" s="6"/>
       <c r="C20" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D20" s="1"/>
+        <v>20</v>
+      </c>
+      <c r="D20" s="4"/>
       <c r="E20" s="1"/>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="21" spans="1:5">
       <c r="A21" s="7"/>
       <c r="B21" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D21" s="1"/>
+        <v>23</v>
+      </c>
+      <c r="D21" s="4"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="22" spans="1:5">
       <c r="A22" s="7"/>
       <c r="B22" s="2" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D22" s="1"/>
+        <v>71</v>
+      </c>
+      <c r="D22" s="5"/>
       <c r="E22" s="1"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="23" spans="1:5">
       <c r="A23" s="7"/>
       <c r="B23" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D23" s="1"/>
+      <c r="D23" s="4"/>
       <c r="E23" s="1"/>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="24" spans="1:5">
       <c r="A24" s="7"/>
       <c r="B24" s="6"/>
       <c r="C24" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D24" s="1"/>
+      <c r="D24" s="4"/>
       <c r="E24" s="1"/>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="25" spans="1:5">
       <c r="A25" s="7"/>
       <c r="B25" s="6"/>
       <c r="C25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="1"/>
+      <c r="D25" s="4"/>
       <c r="E25" s="1"/>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="26" spans="1:5">
       <c r="A26" s="7"/>
       <c r="B26" s="6"/>
       <c r="C26" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="D26" s="1"/>
+        <v>56</v>
+      </c>
+      <c r="D26" s="4"/>
       <c r="E26" s="1"/>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A27" s="9">
+    <row r="27" spans="1:5" ht="77.25" customHeight="1">
+      <c r="A27" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10"/>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" s="12">
         <v>42130</v>
       </c>
-      <c r="B27" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A28" s="10"/>
-      <c r="B28" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>32</v>
+      <c r="B28" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A29" s="10"/>
-      <c r="B29" s="6"/>
-      <c r="C29" s="4" t="s">
-        <v>31</v>
+    <row r="29" spans="1:5">
+      <c r="A29" s="13"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="1" t="s">
+        <v>67</v>
       </c>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A30" s="10"/>
-      <c r="B30" s="6"/>
-      <c r="C30" s="4" t="s">
-        <v>33</v>
+    <row r="30" spans="1:5">
+      <c r="A30" s="13"/>
+      <c r="B30" s="17"/>
+      <c r="C30" s="1" t="s">
+        <v>68</v>
       </c>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A31" s="10"/>
-      <c r="B31" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>35</v>
+    <row r="31" spans="1:5">
+      <c r="A31" s="13"/>
+      <c r="B31" s="18"/>
+      <c r="C31" s="1" t="s">
+        <v>69</v>
       </c>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A32" s="10"/>
-      <c r="B32" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>37</v>
+    <row r="32" spans="1:5">
+      <c r="A32" s="13"/>
+      <c r="B32" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A33" s="10"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="4" t="s">
-        <v>38</v>
+    <row r="33" spans="1:5">
+      <c r="A33" s="13"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A34" s="10"/>
-      <c r="B34" s="8"/>
-      <c r="C34" s="4" t="s">
-        <v>39</v>
+    <row r="34" spans="1:5">
+      <c r="A34" s="13"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="3" t="s">
+        <v>30</v>
       </c>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A35" s="11"/>
-      <c r="B35" s="8"/>
-      <c r="C35" s="4" t="s">
-        <v>40</v>
+    <row r="35" spans="1:5">
+      <c r="A35" s="13"/>
+      <c r="B35" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>72</v>
       </c>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A36" s="7">
-        <v>42131</v>
-      </c>
-      <c r="B36" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>42</v>
+    <row r="36" spans="1:5">
+      <c r="A36" s="13"/>
+      <c r="B36" s="20"/>
+      <c r="C36" s="3" t="s">
+        <v>32</v>
       </c>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A37" s="7"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="4" t="s">
-        <v>43</v>
+    <row r="37" spans="1:5">
+      <c r="A37" s="13"/>
+      <c r="B37" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>34</v>
       </c>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A38" s="7"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="4" t="s">
-        <v>44</v>
+    <row r="38" spans="1:5">
+      <c r="A38" s="13"/>
+      <c r="B38" s="11"/>
+      <c r="C38" s="3" t="s">
+        <v>35</v>
       </c>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A39" s="7"/>
-      <c r="B39" s="6"/>
-      <c r="C39" s="4" t="s">
-        <v>45</v>
+    <row r="39" spans="1:5">
+      <c r="A39" s="13"/>
+      <c r="B39" s="11"/>
+      <c r="C39" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A40" s="7"/>
-      <c r="B40" s="6"/>
-      <c r="C40" s="4" t="s">
-        <v>46</v>
+    <row r="40" spans="1:5">
+      <c r="A40" s="14"/>
+      <c r="B40" s="11"/>
+      <c r="C40" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A41" s="7"/>
+    <row r="41" spans="1:5">
+      <c r="A41" s="7">
+        <v>42131</v>
+      </c>
       <c r="B41" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>48</v>
+        <v>38</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>39</v>
       </c>
       <c r="D41" s="1"/>
       <c r="E41" s="1"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="42" spans="1:5">
       <c r="A42" s="7"/>
       <c r="B42" s="6"/>
-      <c r="C42" s="4" t="s">
-        <v>49</v>
+      <c r="C42" s="3" t="s">
+        <v>40</v>
       </c>
       <c r="D42" s="1"/>
       <c r="E42" s="1"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="43" spans="1:5">
       <c r="A43" s="7"/>
-      <c r="B43" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>51</v>
+      <c r="B43" s="6"/>
+      <c r="C43" s="3" t="s">
+        <v>41</v>
       </c>
       <c r="D43" s="1"/>
       <c r="E43" s="1"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="44" spans="1:5">
       <c r="A44" s="7"/>
       <c r="B44" s="6"/>
-      <c r="C44" s="4" t="s">
-        <v>50</v>
+      <c r="C44" s="3" t="s">
+        <v>42</v>
       </c>
       <c r="D44" s="1"/>
       <c r="E44" s="1"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="45" spans="1:5">
       <c r="A45" s="7"/>
-      <c r="B45" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>52</v>
+      <c r="B45" s="6"/>
+      <c r="C45" s="3" t="s">
+        <v>43</v>
       </c>
       <c r="D45" s="1"/>
       <c r="E45" s="1"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A46" s="7">
-        <v>42132</v>
-      </c>
+    <row r="46" spans="1:5">
+      <c r="A46" s="7"/>
       <c r="B46" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>54</v>
+        <v>44</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="D46" s="1"/>
       <c r="E46" s="1"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="47" spans="1:5">
       <c r="A47" s="7"/>
       <c r="B47" s="6"/>
-      <c r="C47" s="4" t="s">
-        <v>55</v>
+      <c r="C47" s="3" t="s">
+        <v>46</v>
       </c>
       <c r="D47" s="1"/>
       <c r="E47" s="1"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="48" spans="1:5">
       <c r="A48" s="7"/>
-      <c r="B48" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>57</v>
+      <c r="B48" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C48" s="3" t="s">
+        <v>48</v>
       </c>
       <c r="D48" s="1"/>
       <c r="E48" s="1"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="49" spans="1:5">
       <c r="A49" s="7"/>
-      <c r="B49" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C49" s="4" t="s">
-        <v>55</v>
+      <c r="B49" s="6"/>
+      <c r="C49" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="D49" s="1"/>
       <c r="E49" s="1"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="50" spans="1:5">
       <c r="A50" s="7"/>
-      <c r="B50" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>60</v>
+      <c r="B50" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>49</v>
       </c>
       <c r="D50" s="1"/>
       <c r="E50" s="1"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="A51" s="7"/>
-      <c r="B51" s="6"/>
-      <c r="C51" s="4" t="s">
-        <v>61</v>
+    <row r="51" spans="1:5">
+      <c r="A51" s="7">
+        <v>42132</v>
+      </c>
+      <c r="B51" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>51</v>
       </c>
       <c r="D51" s="1"/>
       <c r="E51" s="1"/>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="52" spans="1:5">
       <c r="A52" s="7"/>
       <c r="B52" s="6"/>
-      <c r="C52" s="4" t="s">
-        <v>62</v>
+      <c r="C52" s="3" t="s">
+        <v>52</v>
       </c>
       <c r="D52" s="1"/>
       <c r="E52" s="1"/>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.15">
+    <row r="53" spans="1:5">
       <c r="A53" s="7"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="4" t="s">
-        <v>63</v>
+      <c r="B53" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
     </row>
+    <row r="54" spans="1:5">
+      <c r="A54" s="7"/>
+      <c r="B54" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D54" s="1"/>
+      <c r="E54" s="1"/>
+    </row>
+    <row r="55" spans="1:5">
+      <c r="A55" s="7"/>
+      <c r="B55" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D55" s="1"/>
+      <c r="E55" s="1"/>
+    </row>
+    <row r="56" spans="1:5">
+      <c r="A56" s="7"/>
+      <c r="B56" s="6"/>
+      <c r="C56" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D56" s="1"/>
+      <c r="E56" s="1"/>
+    </row>
+    <row r="57" spans="1:5">
+      <c r="A57" s="7"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D57" s="1"/>
+      <c r="E57" s="1"/>
+    </row>
+    <row r="58" spans="1:5">
+      <c r="A58" s="7"/>
+      <c r="B58" s="6"/>
+      <c r="C58" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="D58" s="1"/>
+      <c r="E58" s="1"/>
+    </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="20">
+    <mergeCell ref="A27:E27"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="A41:A50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="B55:B58"/>
+    <mergeCell ref="A51:A58"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="B37:B40"/>
+    <mergeCell ref="A28:A40"/>
+    <mergeCell ref="B41:B45"/>
+    <mergeCell ref="B46:B47"/>
     <mergeCell ref="B2:B6"/>
     <mergeCell ref="B9:B11"/>
     <mergeCell ref="A2:A11"/>
@@ -1363,16 +1522,6 @@
     <mergeCell ref="B23:B26"/>
     <mergeCell ref="A13:A26"/>
     <mergeCell ref="A12:E12"/>
-    <mergeCell ref="B28:B30"/>
-    <mergeCell ref="B32:B35"/>
-    <mergeCell ref="A27:A35"/>
-    <mergeCell ref="B36:B40"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A36:A45"/>
-    <mergeCell ref="B46:B47"/>
-    <mergeCell ref="B50:B53"/>
-    <mergeCell ref="A46:A53"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1386,7 +1535,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1399,7 +1548,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <sheetData/>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update Map Logic & Models
FXXK YOU System.Data.dll
</commit_message>
<xml_diff>
--- a/Docs/UniBOOM_Checklist.xlsx
+++ b/Docs/UniBOOM_Checklist.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="195">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="197">
   <si>
     <t>日期</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -439,10 +439,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>BigTree</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>完成赛博风地板模型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -499,10 +495,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>检查地图自动生成逻辑</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>完善地图自动生成逻辑</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -511,23 +503,7 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>UI要素制作（待定）</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>完善赛博风怪物模型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>完善RPG场景模型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成“摄像头”模型</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>完成“机械狗”模型</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -890,6 +866,39 @@
 地图数据结构暂且考虑了下，但是还没写下来。
 BigTree八成是忘了。
 天空盒素材暂时不打紧，先把中心放在动画制作上。</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完善地图自动生成逻辑</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>制作选关界面UI</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完善游戏界面UI要素</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>完善logo</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>制作“气球”动画</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>制作“锅”动画</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>制作“小花”动画</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>地图自动生成逻辑遇到问题，延误了进度。
+Dog居然什么都没做。</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1080,7 +1089,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1144,6 +1153,54 @@
     <xf numFmtId="58" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="58" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1153,59 +1210,14 @@
     <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="58" fontId="2" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="58" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1508,10 +1520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E306"/>
+  <dimension ref="A1:E312"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A120" sqref="A120:A125"/>
+    <sheetView tabSelected="1" topLeftCell="A121" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A132" sqref="A132:E132"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -1544,7 +1556,7 @@
       <c r="A2" s="24">
         <v>42128</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C2" s="1" t="s">
@@ -1557,7 +1569,7 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="24"/>
-      <c r="B3" s="25"/>
+      <c r="B3" s="23"/>
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
@@ -1568,7 +1580,7 @@
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="24"/>
-      <c r="B4" s="25"/>
+      <c r="B4" s="23"/>
       <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
@@ -1579,7 +1591,7 @@
     </row>
     <row r="5" spans="1:5">
       <c r="A5" s="24"/>
-      <c r="B5" s="25"/>
+      <c r="B5" s="23"/>
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
@@ -1590,7 +1602,7 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="24"/>
-      <c r="B6" s="25"/>
+      <c r="B6" s="23"/>
       <c r="C6" s="1" t="s">
         <v>19</v>
       </c>
@@ -1621,7 +1633,7 @@
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="24"/>
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="23" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -1632,7 +1644,7 @@
     </row>
     <row r="10" spans="1:5">
       <c r="A10" s="24"/>
-      <c r="B10" s="25"/>
+      <c r="B10" s="23"/>
       <c r="C10" s="1" t="s">
         <v>14</v>
       </c>
@@ -1641,7 +1653,7 @@
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="24"/>
-      <c r="B11" s="25"/>
+      <c r="B11" s="23"/>
       <c r="C11" s="1" t="s">
         <v>15</v>
       </c>
@@ -1649,19 +1661,19 @@
       <c r="E11" s="1"/>
     </row>
     <row r="12" spans="1:5" ht="49.5" customHeight="1">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="25" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="30"/>
-      <c r="C12" s="30"/>
-      <c r="D12" s="30"/>
-      <c r="E12" s="31"/>
+      <c r="B12" s="34"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="35"/>
     </row>
     <row r="13" spans="1:5">
       <c r="A13" s="24">
         <v>42129</v>
       </c>
-      <c r="B13" s="25" t="s">
+      <c r="B13" s="23" t="s">
         <v>5</v>
       </c>
       <c r="C13" s="1" t="s">
@@ -1669,12 +1681,12 @@
       </c>
       <c r="D13" s="4"/>
       <c r="E13" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="14" spans="1:5">
       <c r="A14" s="24"/>
-      <c r="B14" s="25"/>
+      <c r="B14" s="23"/>
       <c r="C14" s="1" t="s">
         <v>51</v>
       </c>
@@ -1685,7 +1697,7 @@
     </row>
     <row r="15" spans="1:5">
       <c r="A15" s="24"/>
-      <c r="B15" s="25"/>
+      <c r="B15" s="23"/>
       <c r="C15" s="1" t="s">
         <v>25</v>
       </c>
@@ -1696,7 +1708,7 @@
     </row>
     <row r="16" spans="1:5">
       <c r="A16" s="24"/>
-      <c r="B16" s="25"/>
+      <c r="B16" s="23"/>
       <c r="C16" s="1" t="s">
         <v>17</v>
       </c>
@@ -1707,7 +1719,7 @@
     </row>
     <row r="17" spans="1:5">
       <c r="A17" s="24"/>
-      <c r="B17" s="25"/>
+      <c r="B17" s="23"/>
       <c r="C17" s="1" t="s">
         <v>57</v>
       </c>
@@ -1716,7 +1728,7 @@
     </row>
     <row r="18" spans="1:5">
       <c r="A18" s="24"/>
-      <c r="B18" s="25"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="1" t="s">
         <v>58</v>
       </c>
@@ -1725,7 +1737,7 @@
     </row>
     <row r="19" spans="1:5">
       <c r="A19" s="24"/>
-      <c r="B19" s="25"/>
+      <c r="B19" s="23"/>
       <c r="C19" s="1" t="s">
         <v>59</v>
       </c>
@@ -1734,7 +1746,7 @@
     </row>
     <row r="20" spans="1:5">
       <c r="A20" s="24"/>
-      <c r="B20" s="25"/>
+      <c r="B20" s="23"/>
       <c r="C20" s="1" t="s">
         <v>64</v>
       </c>
@@ -1743,7 +1755,7 @@
     </row>
     <row r="21" spans="1:5">
       <c r="A21" s="24"/>
-      <c r="B21" s="25"/>
+      <c r="B21" s="23"/>
       <c r="C21" s="1" t="s">
         <v>20</v>
       </c>
@@ -1774,7 +1786,7 @@
     </row>
     <row r="24" spans="1:5">
       <c r="A24" s="24"/>
-      <c r="B24" s="25" t="s">
+      <c r="B24" s="23" t="s">
         <v>24</v>
       </c>
       <c r="C24" s="1" t="s">
@@ -1785,7 +1797,7 @@
     </row>
     <row r="25" spans="1:5">
       <c r="A25" s="24"/>
-      <c r="B25" s="25"/>
+      <c r="B25" s="23"/>
       <c r="C25" s="1" t="s">
         <v>14</v>
       </c>
@@ -1794,7 +1806,7 @@
     </row>
     <row r="26" spans="1:5">
       <c r="A26" s="24"/>
-      <c r="B26" s="25"/>
+      <c r="B26" s="23"/>
       <c r="C26" s="1" t="s">
         <v>15</v>
       </c>
@@ -1803,7 +1815,7 @@
     </row>
     <row r="27" spans="1:5">
       <c r="A27" s="24"/>
-      <c r="B27" s="25"/>
+      <c r="B27" s="23"/>
       <c r="C27" s="3" t="s">
         <v>48</v>
       </c>
@@ -1811,19 +1823,19 @@
       <c r="E27" s="1"/>
     </row>
     <row r="28" spans="1:5" ht="77.25" customHeight="1">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="30"/>
-      <c r="E28" s="31"/>
+      <c r="B28" s="34"/>
+      <c r="C28" s="34"/>
+      <c r="D28" s="34"/>
+      <c r="E28" s="35"/>
     </row>
     <row r="29" spans="1:5">
       <c r="A29" s="18">
         <v>42130</v>
       </c>
-      <c r="B29" s="33" t="s">
+      <c r="B29" s="30" t="s">
         <v>26</v>
       </c>
       <c r="C29" s="3" t="s">
@@ -1834,40 +1846,40 @@
     </row>
     <row r="30" spans="1:5">
       <c r="A30" s="19"/>
-      <c r="B30" s="36"/>
+      <c r="B30" s="31"/>
       <c r="C30" s="3" t="s">
         <v>74</v>
       </c>
       <c r="D30" s="4"/>
       <c r="E30" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="31" spans="1:5">
       <c r="A31" s="19"/>
-      <c r="B31" s="36"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="7" t="s">
         <v>75</v>
       </c>
       <c r="D31" s="4"/>
       <c r="E31" s="1" t="s">
-        <v>122</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" spans="1:5">
       <c r="A32" s="19"/>
-      <c r="B32" s="36"/>
+      <c r="B32" s="31"/>
       <c r="C32" s="1" t="s">
         <v>57</v>
       </c>
       <c r="D32" s="4"/>
       <c r="E32" s="1" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="33" spans="1:5">
       <c r="A33" s="19"/>
-      <c r="B33" s="36"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="1" t="s">
         <v>58</v>
       </c>
@@ -1876,18 +1888,18 @@
     </row>
     <row r="34" spans="1:5">
       <c r="A34" s="19"/>
-      <c r="B34" s="36"/>
+      <c r="B34" s="31"/>
       <c r="C34" s="1" t="s">
         <v>59</v>
       </c>
       <c r="D34" s="4"/>
       <c r="E34" s="1" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="35" spans="1:5">
       <c r="A35" s="19"/>
-      <c r="B35" s="36"/>
+      <c r="B35" s="31"/>
       <c r="C35" s="3" t="s">
         <v>69</v>
       </c>
@@ -1896,7 +1908,7 @@
     </row>
     <row r="36" spans="1:5">
       <c r="A36" s="19"/>
-      <c r="B36" s="34"/>
+      <c r="B36" s="32"/>
       <c r="C36" s="7" t="s">
         <v>62</v>
       </c>
@@ -1916,7 +1928,7 @@
     </row>
     <row r="38" spans="1:5">
       <c r="A38" s="19"/>
-      <c r="B38" s="37" t="s">
+      <c r="B38" s="28" t="s">
         <v>28</v>
       </c>
       <c r="C38" s="3" t="s">
@@ -1927,7 +1939,7 @@
     </row>
     <row r="39" spans="1:5">
       <c r="A39" s="19"/>
-      <c r="B39" s="38"/>
+      <c r="B39" s="36"/>
       <c r="C39" s="3" t="s">
         <v>29</v>
       </c>
@@ -1936,7 +1948,7 @@
     </row>
     <row r="40" spans="1:5">
       <c r="A40" s="19"/>
-      <c r="B40" s="32" t="s">
+      <c r="B40" s="21" t="s">
         <v>30</v>
       </c>
       <c r="C40" s="3" t="s">
@@ -1944,45 +1956,45 @@
       </c>
       <c r="D40" s="4"/>
       <c r="E40" s="1" t="s">
-        <v>123</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:5">
       <c r="A41" s="19"/>
-      <c r="B41" s="32"/>
+      <c r="B41" s="21"/>
       <c r="C41" s="3" t="s">
         <v>32</v>
       </c>
       <c r="D41" s="4"/>
       <c r="E41" s="1" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:5">
       <c r="A42" s="19"/>
-      <c r="B42" s="32"/>
+      <c r="B42" s="21"/>
       <c r="C42" s="3" t="s">
         <v>33</v>
       </c>
       <c r="D42" s="4"/>
       <c r="E42" s="1" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:5">
       <c r="A43" s="19"/>
-      <c r="B43" s="32"/>
+      <c r="B43" s="21"/>
       <c r="C43" s="3" t="s">
         <v>34</v>
       </c>
       <c r="D43" s="4"/>
       <c r="E43" s="1" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:5">
       <c r="A44" s="19"/>
-      <c r="B44" s="37" t="s">
+      <c r="B44" s="28" t="s">
         <v>88</v>
       </c>
       <c r="C44" s="3" t="s">
@@ -1990,34 +2002,34 @@
       </c>
       <c r="D44" s="4"/>
       <c r="E44" s="1" t="s">
-        <v>127</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:5">
       <c r="A45" s="20"/>
-      <c r="B45" s="38"/>
+      <c r="B45" s="36"/>
       <c r="C45" s="3" t="s">
         <v>83</v>
       </c>
       <c r="D45" s="5"/>
       <c r="E45" s="1" t="s">
-        <v>128</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:5" ht="107.25" customHeight="1">
-      <c r="A46" s="29" t="s">
-        <v>130</v>
-      </c>
-      <c r="B46" s="39"/>
-      <c r="C46" s="39"/>
-      <c r="D46" s="39"/>
-      <c r="E46" s="40"/>
+      <c r="A46" s="25" t="s">
+        <v>124</v>
+      </c>
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="D46" s="26"/>
+      <c r="E46" s="27"/>
     </row>
     <row r="47" spans="1:5">
       <c r="A47" s="18">
         <v>42131</v>
       </c>
-      <c r="B47" s="25" t="s">
+      <c r="B47" s="23" t="s">
         <v>35</v>
       </c>
       <c r="C47" s="3" t="s">
@@ -2028,7 +2040,7 @@
     </row>
     <row r="48" spans="1:5">
       <c r="A48" s="19"/>
-      <c r="B48" s="25"/>
+      <c r="B48" s="23"/>
       <c r="C48" s="3" t="s">
         <v>37</v>
       </c>
@@ -2037,7 +2049,7 @@
     </row>
     <row r="49" spans="1:5">
       <c r="A49" s="19"/>
-      <c r="B49" s="25"/>
+      <c r="B49" s="23"/>
       <c r="C49" s="3" t="s">
         <v>38</v>
       </c>
@@ -2046,7 +2058,7 @@
     </row>
     <row r="50" spans="1:5">
       <c r="A50" s="19"/>
-      <c r="B50" s="25"/>
+      <c r="B50" s="23"/>
       <c r="C50" s="3" t="s">
         <v>39</v>
       </c>
@@ -2055,7 +2067,7 @@
     </row>
     <row r="51" spans="1:5">
       <c r="A51" s="19"/>
-      <c r="B51" s="25"/>
+      <c r="B51" s="23"/>
       <c r="C51" s="3" t="s">
         <v>40</v>
       </c>
@@ -2064,16 +2076,16 @@
     </row>
     <row r="52" spans="1:5">
       <c r="A52" s="19"/>
-      <c r="B52" s="25"/>
+      <c r="B52" s="23"/>
       <c r="C52" s="3" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
       <c r="D52" s="4"/>
       <c r="E52" s="1"/>
     </row>
     <row r="53" spans="1:5">
       <c r="A53" s="19"/>
-      <c r="B53" s="25"/>
+      <c r="B53" s="23"/>
       <c r="C53" s="1" t="s">
         <v>58</v>
       </c>
@@ -2086,14 +2098,14 @@
         <v>41</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D54" s="5"/>
       <c r="E54" s="1"/>
     </row>
     <row r="55" spans="1:5">
       <c r="A55" s="19"/>
-      <c r="B55" s="25" t="s">
+      <c r="B55" s="23" t="s">
         <v>10</v>
       </c>
       <c r="C55" s="3" t="s">
@@ -2104,7 +2116,7 @@
     </row>
     <row r="56" spans="1:5">
       <c r="A56" s="19"/>
-      <c r="B56" s="25"/>
+      <c r="B56" s="23"/>
       <c r="C56" s="3" t="s">
         <v>42</v>
       </c>
@@ -2113,18 +2125,18 @@
     </row>
     <row r="57" spans="1:5">
       <c r="A57" s="19"/>
-      <c r="B57" s="33" t="s">
+      <c r="B57" s="30" t="s">
         <v>30</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="D57" s="4"/>
       <c r="E57" s="1"/>
     </row>
     <row r="58" spans="1:5">
       <c r="A58" s="19"/>
-      <c r="B58" s="34"/>
+      <c r="B58" s="32"/>
       <c r="C58" s="3" t="s">
         <v>72</v>
       </c>
@@ -2133,7 +2145,7 @@
     </row>
     <row r="59" spans="1:5">
       <c r="A59" s="19"/>
-      <c r="B59" s="37" t="s">
+      <c r="B59" s="28" t="s">
         <v>88</v>
       </c>
       <c r="C59" s="3" t="s">
@@ -2144,7 +2156,7 @@
     </row>
     <row r="60" spans="1:5">
       <c r="A60" s="20"/>
-      <c r="B60" s="38"/>
+      <c r="B60" s="36"/>
       <c r="C60" s="3" t="s">
         <v>50</v>
       </c>
@@ -2152,19 +2164,19 @@
       <c r="E60" s="1"/>
     </row>
     <row r="61" spans="1:5" ht="48" customHeight="1">
-      <c r="A61" s="29" t="s">
-        <v>186</v>
-      </c>
-      <c r="B61" s="39"/>
-      <c r="C61" s="39"/>
-      <c r="D61" s="39"/>
-      <c r="E61" s="40"/>
+      <c r="A61" s="25" t="s">
+        <v>180</v>
+      </c>
+      <c r="B61" s="26"/>
+      <c r="C61" s="26"/>
+      <c r="D61" s="26"/>
+      <c r="E61" s="27"/>
     </row>
     <row r="62" spans="1:5">
       <c r="A62" s="18">
         <v>42132</v>
       </c>
-      <c r="B62" s="25" t="s">
+      <c r="B62" s="23" t="s">
         <v>44</v>
       </c>
       <c r="C62" s="3" t="s">
@@ -2175,16 +2187,16 @@
     </row>
     <row r="63" spans="1:5">
       <c r="A63" s="19"/>
-      <c r="B63" s="25"/>
+      <c r="B63" s="23"/>
       <c r="C63" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D63" s="5"/>
       <c r="E63" s="1"/>
     </row>
     <row r="64" spans="1:5">
       <c r="A64" s="19"/>
-      <c r="B64" s="25"/>
+      <c r="B64" s="23"/>
       <c r="C64" s="3" t="s">
         <v>36</v>
       </c>
@@ -2193,7 +2205,7 @@
     </row>
     <row r="65" spans="1:5">
       <c r="A65" s="19"/>
-      <c r="B65" s="25"/>
+      <c r="B65" s="23"/>
       <c r="C65" s="3" t="s">
         <v>37</v>
       </c>
@@ -2202,7 +2214,7 @@
     </row>
     <row r="66" spans="1:5">
       <c r="A66" s="19"/>
-      <c r="B66" s="25"/>
+      <c r="B66" s="23"/>
       <c r="C66" s="3" t="s">
         <v>38</v>
       </c>
@@ -2211,7 +2223,7 @@
     </row>
     <row r="67" spans="1:5">
       <c r="A67" s="19"/>
-      <c r="B67" s="25"/>
+      <c r="B67" s="23"/>
       <c r="C67" s="3" t="s">
         <v>39</v>
       </c>
@@ -2220,7 +2232,7 @@
     </row>
     <row r="68" spans="1:5">
       <c r="A68" s="19"/>
-      <c r="B68" s="25"/>
+      <c r="B68" s="23"/>
       <c r="C68" s="3" t="s">
         <v>40</v>
       </c>
@@ -2229,7 +2241,7 @@
     </row>
     <row r="69" spans="1:5">
       <c r="A69" s="19"/>
-      <c r="B69" s="25"/>
+      <c r="B69" s="23"/>
       <c r="C69" s="1" t="s">
         <v>58</v>
       </c>
@@ -2242,7 +2254,7 @@
         <v>46</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="D70" s="4"/>
       <c r="E70" s="1"/>
@@ -2253,25 +2265,25 @@
         <v>47</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>131</v>
+        <v>125</v>
       </c>
       <c r="D71" s="4"/>
       <c r="E71" s="1"/>
     </row>
     <row r="72" spans="1:5">
       <c r="A72" s="19"/>
-      <c r="B72" s="33" t="s">
+      <c r="B72" s="30" t="s">
         <v>84</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D72" s="4"/>
       <c r="E72" s="1"/>
     </row>
     <row r="73" spans="1:5">
       <c r="A73" s="19"/>
-      <c r="B73" s="36"/>
+      <c r="B73" s="31"/>
       <c r="C73" s="3" t="s">
         <v>85</v>
       </c>
@@ -2280,7 +2292,7 @@
     </row>
     <row r="74" spans="1:5">
       <c r="A74" s="19"/>
-      <c r="B74" s="36"/>
+      <c r="B74" s="31"/>
       <c r="C74" s="3" t="s">
         <v>86</v>
       </c>
@@ -2289,7 +2301,7 @@
     </row>
     <row r="75" spans="1:5">
       <c r="A75" s="19"/>
-      <c r="B75" s="34"/>
+      <c r="B75" s="32"/>
       <c r="C75" s="3" t="s">
         <v>87</v>
       </c>
@@ -2298,7 +2310,7 @@
     </row>
     <row r="76" spans="1:5">
       <c r="A76" s="19"/>
-      <c r="B76" s="33" t="s">
+      <c r="B76" s="30" t="s">
         <v>89</v>
       </c>
       <c r="C76" s="3" t="s">
@@ -2309,57 +2321,57 @@
     </row>
     <row r="77" spans="1:5">
       <c r="A77" s="19"/>
-      <c r="B77" s="36"/>
+      <c r="B77" s="31"/>
       <c r="C77" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D77" s="4"/>
       <c r="E77" s="1"/>
     </row>
     <row r="78" spans="1:5">
       <c r="A78" s="19"/>
-      <c r="B78" s="36"/>
+      <c r="B78" s="31"/>
       <c r="C78" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="D78" s="4"/>
       <c r="E78" s="1"/>
     </row>
     <row r="79" spans="1:5">
       <c r="A79" s="19"/>
-      <c r="B79" s="36"/>
+      <c r="B79" s="31"/>
       <c r="C79" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="D79" s="4"/>
       <c r="E79" s="1"/>
     </row>
     <row r="80" spans="1:5">
       <c r="A80" s="19"/>
-      <c r="B80" s="36"/>
+      <c r="B80" s="31"/>
       <c r="C80" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D80" s="17"/>
       <c r="E80" s="12"/>
     </row>
     <row r="81" spans="1:5">
       <c r="A81" s="19"/>
-      <c r="B81" s="36"/>
+      <c r="B81" s="31"/>
       <c r="C81" s="3" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
       <c r="D81" s="17"/>
       <c r="E81" s="12"/>
     </row>
     <row r="82" spans="1:5" ht="42" customHeight="1">
-      <c r="A82" s="29" t="s">
-        <v>187</v>
-      </c>
-      <c r="B82" s="39"/>
-      <c r="C82" s="39"/>
-      <c r="D82" s="39"/>
-      <c r="E82" s="40"/>
+      <c r="A82" s="25" t="s">
+        <v>181</v>
+      </c>
+      <c r="B82" s="26"/>
+      <c r="C82" s="26"/>
+      <c r="D82" s="26"/>
+      <c r="E82" s="27"/>
     </row>
     <row r="83" spans="1:5" ht="13.5" customHeight="1">
       <c r="A83" s="18">
@@ -2419,11 +2431,11 @@
       <c r="E87" s="1"/>
     </row>
     <row r="88" spans="1:5">
-      <c r="A88" s="21"/>
-      <c r="B88" s="22"/>
-      <c r="C88" s="22"/>
-      <c r="D88" s="22"/>
-      <c r="E88" s="23"/>
+      <c r="A88" s="37"/>
+      <c r="B88" s="38"/>
+      <c r="C88" s="38"/>
+      <c r="D88" s="38"/>
+      <c r="E88" s="39"/>
     </row>
     <row r="89" spans="1:5">
       <c r="A89" s="18">
@@ -2483,17 +2495,17 @@
       <c r="E93" s="1"/>
     </row>
     <row r="94" spans="1:5">
-      <c r="A94" s="21"/>
-      <c r="B94" s="22"/>
-      <c r="C94" s="22"/>
-      <c r="D94" s="22"/>
-      <c r="E94" s="23"/>
+      <c r="A94" s="37"/>
+      <c r="B94" s="38"/>
+      <c r="C94" s="38"/>
+      <c r="D94" s="38"/>
+      <c r="E94" s="39"/>
     </row>
     <row r="95" spans="1:5">
       <c r="A95" s="24">
         <v>42135</v>
       </c>
-      <c r="B95" s="32" t="s">
+      <c r="B95" s="21" t="s">
         <v>71</v>
       </c>
       <c r="C95" s="3" t="s">
@@ -2504,7 +2516,7 @@
     </row>
     <row r="96" spans="1:5">
       <c r="A96" s="24"/>
-      <c r="B96" s="32"/>
+      <c r="B96" s="21"/>
       <c r="C96" s="3" t="s">
         <v>73</v>
       </c>
@@ -2513,52 +2525,52 @@
     </row>
     <row r="97" spans="1:5">
       <c r="A97" s="24"/>
-      <c r="B97" s="32"/>
+      <c r="B97" s="21"/>
       <c r="C97" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D97" s="4"/>
       <c r="E97" s="1"/>
     </row>
     <row r="98" spans="1:5">
       <c r="A98" s="24"/>
-      <c r="B98" s="32"/>
+      <c r="B98" s="21"/>
       <c r="C98" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="D98" s="4"/>
       <c r="E98" s="1"/>
     </row>
     <row r="99" spans="1:5">
       <c r="A99" s="24"/>
-      <c r="B99" s="32"/>
+      <c r="B99" s="21"/>
       <c r="C99" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D99" s="4"/>
       <c r="E99" s="1"/>
     </row>
     <row r="100" spans="1:5">
       <c r="A100" s="24"/>
-      <c r="B100" s="32"/>
+      <c r="B100" s="21"/>
       <c r="C100" s="3" t="s">
-        <v>188</v>
+        <v>182</v>
       </c>
       <c r="D100" s="4"/>
       <c r="E100" s="1"/>
     </row>
     <row r="101" spans="1:5">
       <c r="A101" s="24"/>
-      <c r="B101" s="32"/>
+      <c r="B101" s="21"/>
       <c r="C101" s="7" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="D101" s="4"/>
       <c r="E101" s="1"/>
     </row>
     <row r="102" spans="1:5">
       <c r="A102" s="24"/>
-      <c r="B102" s="32"/>
+      <c r="B102" s="21"/>
       <c r="C102" s="3" t="s">
         <v>38</v>
       </c>
@@ -2567,7 +2579,7 @@
     </row>
     <row r="103" spans="1:5">
       <c r="A103" s="24"/>
-      <c r="B103" s="32"/>
+      <c r="B103" s="21"/>
       <c r="C103" s="3" t="s">
         <v>40</v>
       </c>
@@ -2576,7 +2588,7 @@
     </row>
     <row r="104" spans="1:5">
       <c r="A104" s="24"/>
-      <c r="B104" s="32"/>
+      <c r="B104" s="21"/>
       <c r="C104" s="1" t="s">
         <v>58</v>
       </c>
@@ -2585,7 +2597,7 @@
     </row>
     <row r="105" spans="1:5">
       <c r="A105" s="24"/>
-      <c r="B105" s="32" t="s">
+      <c r="B105" s="21" t="s">
         <v>76</v>
       </c>
       <c r="C105" s="3" t="s">
@@ -2596,7 +2608,7 @@
     </row>
     <row r="106" spans="1:5">
       <c r="A106" s="24"/>
-      <c r="B106" s="32"/>
+      <c r="B106" s="21"/>
       <c r="C106" s="3" t="s">
         <v>78</v>
       </c>
@@ -2605,7 +2617,7 @@
     </row>
     <row r="107" spans="1:5">
       <c r="A107" s="24"/>
-      <c r="B107" s="32"/>
+      <c r="B107" s="21"/>
       <c r="C107" s="3" t="s">
         <v>79</v>
       </c>
@@ -2614,7 +2626,7 @@
     </row>
     <row r="108" spans="1:5">
       <c r="A108" s="24"/>
-      <c r="B108" s="32"/>
+      <c r="B108" s="21"/>
       <c r="C108" s="3" t="s">
         <v>80</v>
       </c>
@@ -2623,108 +2635,108 @@
     </row>
     <row r="109" spans="1:5">
       <c r="A109" s="24"/>
-      <c r="B109" s="37" t="s">
-        <v>106</v>
+      <c r="B109" s="28" t="s">
+        <v>105</v>
       </c>
       <c r="C109" s="3" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="D109" s="4"/>
       <c r="E109" s="1"/>
     </row>
     <row r="110" spans="1:5">
       <c r="A110" s="24"/>
-      <c r="B110" s="41"/>
+      <c r="B110" s="29"/>
       <c r="C110" s="3" t="s">
-        <v>189</v>
+        <v>183</v>
       </c>
       <c r="D110" s="4"/>
       <c r="E110" s="1"/>
     </row>
     <row r="111" spans="1:5">
       <c r="A111" s="24"/>
-      <c r="B111" s="41"/>
+      <c r="B111" s="29"/>
       <c r="C111" s="3" t="s">
-        <v>191</v>
+        <v>185</v>
       </c>
       <c r="D111" s="4"/>
       <c r="E111" s="1"/>
     </row>
     <row r="112" spans="1:5">
       <c r="A112" s="24"/>
-      <c r="B112" s="25" t="s">
+      <c r="B112" s="23" t="s">
         <v>84</v>
       </c>
       <c r="C112" s="3" t="s">
-        <v>137</v>
+        <v>131</v>
       </c>
       <c r="D112" s="5"/>
       <c r="E112" s="1"/>
     </row>
     <row r="113" spans="1:5">
       <c r="A113" s="24"/>
-      <c r="B113" s="25"/>
+      <c r="B113" s="23"/>
       <c r="C113" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D113" s="5"/>
       <c r="E113" s="1"/>
     </row>
     <row r="114" spans="1:5">
       <c r="A114" s="24"/>
-      <c r="B114" s="25"/>
+      <c r="B114" s="23"/>
       <c r="C114" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D114" s="5"/>
       <c r="E114" s="1"/>
     </row>
     <row r="115" spans="1:5">
       <c r="A115" s="24"/>
-      <c r="B115" s="25"/>
+      <c r="B115" s="23"/>
       <c r="C115" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D115" s="5"/>
       <c r="E115" s="1"/>
     </row>
     <row r="116" spans="1:5">
       <c r="A116" s="24"/>
-      <c r="B116" s="33" t="s">
+      <c r="B116" s="30" t="s">
         <v>89</v>
       </c>
       <c r="C116" s="3" t="s">
-        <v>192</v>
+        <v>186</v>
       </c>
       <c r="D116" s="4"/>
       <c r="E116" s="1"/>
     </row>
     <row r="117" spans="1:5">
       <c r="A117" s="24"/>
-      <c r="B117" s="36"/>
+      <c r="B117" s="31"/>
       <c r="C117" s="3" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="D117" s="4"/>
       <c r="E117" s="1"/>
     </row>
     <row r="118" spans="1:5">
       <c r="A118" s="24"/>
-      <c r="B118" s="34"/>
+      <c r="B118" s="32"/>
       <c r="C118" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D118" s="5"/>
       <c r="E118" s="1"/>
     </row>
     <row r="119" spans="1:5" ht="78" customHeight="1">
-      <c r="A119" s="29" t="s">
-        <v>194</v>
-      </c>
-      <c r="B119" s="39"/>
-      <c r="C119" s="39"/>
-      <c r="D119" s="39"/>
-      <c r="E119" s="40"/>
+      <c r="A119" s="25" t="s">
+        <v>188</v>
+      </c>
+      <c r="B119" s="26"/>
+      <c r="C119" s="26"/>
+      <c r="D119" s="26"/>
+      <c r="E119" s="27"/>
     </row>
     <row r="120" spans="1:5">
       <c r="A120" s="18">
@@ -2734,9 +2746,9 @@
         <v>71</v>
       </c>
       <c r="C120" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="D120" s="1"/>
+        <v>189</v>
+      </c>
+      <c r="D120" s="5"/>
       <c r="E120" s="1"/>
     </row>
     <row r="121" spans="1:5">
@@ -2745,251 +2757,243 @@
         <v>76</v>
       </c>
       <c r="C121" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="D121" s="1"/>
+        <v>107</v>
+      </c>
+      <c r="D121" s="5"/>
       <c r="E121" s="1"/>
     </row>
     <row r="122" spans="1:5">
       <c r="A122" s="19"/>
-      <c r="B122" s="10" t="s">
-        <v>110</v>
+      <c r="B122" s="30" t="s">
+        <v>108</v>
       </c>
       <c r="C122" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D122" s="1"/>
+        <v>190</v>
+      </c>
+      <c r="D122" s="4"/>
       <c r="E122" s="1"/>
     </row>
     <row r="123" spans="1:5">
       <c r="A123" s="19"/>
-      <c r="B123" s="10" t="s">
-        <v>93</v>
-      </c>
+      <c r="B123" s="31"/>
       <c r="C123" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D123" s="1"/>
+        <v>191</v>
+      </c>
+      <c r="D123" s="4"/>
       <c r="E123" s="1"/>
     </row>
     <row r="124" spans="1:5">
       <c r="A124" s="19"/>
-      <c r="B124" s="32" t="s">
+      <c r="B124" s="32"/>
+      <c r="C124" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="D124" s="4"/>
+      <c r="E124" s="1"/>
+    </row>
+    <row r="125" spans="1:5">
+      <c r="A125" s="19"/>
+      <c r="B125" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="C125" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="D125" s="5"/>
+      <c r="E125" s="1"/>
+    </row>
+    <row r="126" spans="1:5">
+      <c r="A126" s="19"/>
+      <c r="B126" s="23"/>
+      <c r="C126" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D126" s="5"/>
+      <c r="E126" s="1"/>
+    </row>
+    <row r="127" spans="1:5">
+      <c r="A127" s="19"/>
+      <c r="B127" s="23"/>
+      <c r="C127" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D127" s="5"/>
+      <c r="E127" s="1"/>
+    </row>
+    <row r="128" spans="1:5">
+      <c r="A128" s="19"/>
+      <c r="B128" s="23"/>
+      <c r="C128" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D128" s="5"/>
+      <c r="E128" s="1"/>
+    </row>
+    <row r="129" spans="1:5">
+      <c r="A129" s="19"/>
+      <c r="B129" s="21" t="s">
         <v>89</v>
       </c>
-      <c r="C124" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="D124" s="1"/>
-      <c r="E124" s="1"/>
-    </row>
-    <row r="125" spans="1:5">
-      <c r="A125" s="20"/>
-      <c r="B125" s="32"/>
-      <c r="C125" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="D125" s="1"/>
-      <c r="E125" s="1"/>
-    </row>
-    <row r="126" spans="1:5">
-      <c r="A126" s="21"/>
-      <c r="B126" s="22"/>
-      <c r="C126" s="22"/>
-      <c r="D126" s="22"/>
-      <c r="E126" s="23"/>
-    </row>
-    <row r="127" spans="1:5">
-      <c r="A127" s="24">
+      <c r="C129" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="D129" s="4"/>
+      <c r="E129" s="1"/>
+    </row>
+    <row r="130" spans="1:5">
+      <c r="A130" s="19"/>
+      <c r="B130" s="21"/>
+      <c r="C130" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="D130" s="4"/>
+      <c r="E130" s="1"/>
+    </row>
+    <row r="131" spans="1:5">
+      <c r="A131" s="20"/>
+      <c r="B131" s="21"/>
+      <c r="C131" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="D131" s="4"/>
+      <c r="E131" s="1"/>
+    </row>
+    <row r="132" spans="1:5" ht="45" customHeight="1">
+      <c r="A132" s="42" t="s">
+        <v>196</v>
+      </c>
+      <c r="B132" s="26"/>
+      <c r="C132" s="26"/>
+      <c r="D132" s="26"/>
+      <c r="E132" s="27"/>
+    </row>
+    <row r="133" spans="1:5">
+      <c r="A133" s="24">
         <v>42137</v>
       </c>
-      <c r="B127" s="28" t="s">
-        <v>116</v>
-      </c>
-      <c r="C127" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="D127" s="1"/>
-      <c r="E127" s="1"/>
-    </row>
-    <row r="128" spans="1:5" ht="409.6">
-      <c r="A128" s="24"/>
-      <c r="B128" s="28"/>
-      <c r="C128" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D128" s="1"/>
-      <c r="E128" s="1"/>
-    </row>
-    <row r="129" spans="1:5">
-      <c r="A129" s="24"/>
-      <c r="B129" s="28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C129" s="3" t="s">
-        <v>118</v>
-      </c>
-      <c r="D129" s="1"/>
-      <c r="E129" s="1"/>
-    </row>
-    <row r="130" spans="1:5">
-      <c r="A130" s="24"/>
-      <c r="B130" s="28"/>
-      <c r="C130" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="D130" s="1"/>
-      <c r="E130" s="1"/>
-    </row>
-    <row r="131" spans="1:5">
-      <c r="A131" s="24"/>
-      <c r="B131" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="C131" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D131" s="1"/>
-      <c r="E131" s="1"/>
-    </row>
-    <row r="132" spans="1:5">
-      <c r="A132" s="24"/>
-      <c r="B132" s="26" t="s">
-        <v>12</v>
-      </c>
-      <c r="C132" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D132" s="1"/>
-      <c r="E132" s="1"/>
-    </row>
-    <row r="133" spans="1:5">
-      <c r="A133" s="24"/>
-      <c r="B133" s="27"/>
+      <c r="B133" s="22" t="s">
+        <v>110</v>
+      </c>
       <c r="C133" s="3" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="D133" s="1"/>
       <c r="E133" s="1"/>
     </row>
     <row r="134" spans="1:5">
       <c r="A134" s="24"/>
-      <c r="B134" s="27"/>
+      <c r="B134" s="22"/>
       <c r="C134" s="3" t="s">
-        <v>136</v>
+        <v>112</v>
       </c>
       <c r="D134" s="1"/>
       <c r="E134" s="1"/>
     </row>
     <row r="135" spans="1:5">
       <c r="A135" s="24"/>
-      <c r="B135" s="27"/>
+      <c r="B135" s="22" t="s">
+        <v>76</v>
+      </c>
       <c r="C135" s="3" t="s">
-        <v>134</v>
+        <v>112</v>
       </c>
       <c r="D135" s="1"/>
       <c r="E135" s="1"/>
     </row>
     <row r="136" spans="1:5">
       <c r="A136" s="24"/>
-      <c r="B136" s="28" t="s">
-        <v>88</v>
-      </c>
+      <c r="B136" s="22"/>
       <c r="C136" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D136" s="1"/>
       <c r="E136" s="1"/>
     </row>
     <row r="137" spans="1:5">
       <c r="A137" s="24"/>
-      <c r="B137" s="28"/>
+      <c r="B137" s="15" t="s">
+        <v>113</v>
+      </c>
       <c r="C137" s="3" t="s">
-        <v>139</v>
+        <v>106</v>
       </c>
       <c r="D137" s="1"/>
       <c r="E137" s="1"/>
     </row>
     <row r="138" spans="1:5">
-      <c r="A138" s="21"/>
-      <c r="B138" s="22"/>
-      <c r="C138" s="22"/>
-      <c r="D138" s="22"/>
-      <c r="E138" s="23"/>
+      <c r="A138" s="24"/>
+      <c r="B138" s="40" t="s">
+        <v>12</v>
+      </c>
+      <c r="C138" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D138" s="1"/>
+      <c r="E138" s="1"/>
     </row>
     <row r="139" spans="1:5">
-      <c r="A139" s="24">
-        <v>42138</v>
-      </c>
-      <c r="B139" s="13" t="s">
-        <v>140</v>
-      </c>
+      <c r="A139" s="24"/>
+      <c r="B139" s="41"/>
       <c r="C139" s="3" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="D139" s="1"/>
       <c r="E139" s="1"/>
     </row>
     <row r="140" spans="1:5">
       <c r="A140" s="24"/>
-      <c r="B140" s="13" t="s">
-        <v>142</v>
-      </c>
+      <c r="B140" s="41"/>
       <c r="C140" s="3" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="D140" s="1"/>
       <c r="E140" s="1"/>
     </row>
     <row r="141" spans="1:5">
       <c r="A141" s="24"/>
-      <c r="B141" s="14" t="s">
-        <v>10</v>
-      </c>
+      <c r="B141" s="41"/>
       <c r="C141" s="3" t="s">
-        <v>107</v>
+        <v>128</v>
       </c>
       <c r="D141" s="1"/>
       <c r="E141" s="1"/>
     </row>
     <row r="142" spans="1:5">
       <c r="A142" s="24"/>
-      <c r="B142" s="14" t="s">
-        <v>147</v>
+      <c r="B142" s="22" t="s">
+        <v>88</v>
       </c>
       <c r="C142" s="3" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D142" s="1"/>
       <c r="E142" s="1"/>
     </row>
     <row r="143" spans="1:5">
       <c r="A143" s="24"/>
-      <c r="B143" s="14" t="s">
-        <v>149</v>
-      </c>
+      <c r="B143" s="22"/>
       <c r="C143" s="3" t="s">
-        <v>153</v>
+        <v>133</v>
       </c>
       <c r="D143" s="1"/>
       <c r="E143" s="1"/>
     </row>
     <row r="144" spans="1:5">
-      <c r="A144" s="21"/>
-      <c r="B144" s="22"/>
-      <c r="C144" s="22"/>
-      <c r="D144" s="22"/>
-      <c r="E144" s="23"/>
+      <c r="A144" s="37"/>
+      <c r="B144" s="38"/>
+      <c r="C144" s="38"/>
+      <c r="D144" s="38"/>
+      <c r="E144" s="39"/>
     </row>
     <row r="145" spans="1:5">
       <c r="A145" s="24">
-        <v>42139</v>
+        <v>42138</v>
       </c>
       <c r="B145" s="13" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="C145" s="3" t="s">
-        <v>150</v>
+        <v>135</v>
       </c>
       <c r="D145" s="1"/>
       <c r="E145" s="1"/>
@@ -2997,10 +3001,10 @@
     <row r="146" spans="1:5">
       <c r="A146" s="24"/>
       <c r="B146" s="13" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="C146" s="3" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D146" s="1"/>
       <c r="E146" s="1"/>
@@ -3011,7 +3015,7 @@
         <v>10</v>
       </c>
       <c r="C147" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D147" s="1"/>
       <c r="E147" s="1"/>
@@ -3019,10 +3023,10 @@
     <row r="148" spans="1:5">
       <c r="A148" s="24"/>
       <c r="B148" s="14" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C148" s="3" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="D148" s="1"/>
       <c r="E148" s="1"/>
@@ -3030,88 +3034,88 @@
     <row r="149" spans="1:5">
       <c r="A149" s="24"/>
       <c r="B149" s="14" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C149" s="3" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="D149" s="1"/>
       <c r="E149" s="1"/>
     </row>
     <row r="150" spans="1:5">
-      <c r="A150" s="25"/>
-      <c r="B150" s="25"/>
-      <c r="C150" s="25"/>
-      <c r="D150" s="25"/>
-      <c r="E150" s="25"/>
+      <c r="A150" s="37"/>
+      <c r="B150" s="38"/>
+      <c r="C150" s="38"/>
+      <c r="D150" s="38"/>
+      <c r="E150" s="39"/>
     </row>
     <row r="151" spans="1:5">
-      <c r="A151" s="18">
-        <v>42140</v>
-      </c>
-      <c r="B151" s="14" t="s">
-        <v>5</v>
+      <c r="A151" s="24">
+        <v>42139</v>
+      </c>
+      <c r="B151" s="13" t="s">
+        <v>134</v>
       </c>
       <c r="C151" s="3" t="s">
-        <v>67</v>
+        <v>144</v>
       </c>
       <c r="D151" s="1"/>
       <c r="E151" s="1"/>
     </row>
     <row r="152" spans="1:5">
-      <c r="A152" s="19"/>
+      <c r="A152" s="24"/>
       <c r="B152" s="13" t="s">
-        <v>9</v>
+        <v>136</v>
       </c>
       <c r="C152" s="3" t="s">
-        <v>67</v>
+        <v>144</v>
       </c>
       <c r="D152" s="1"/>
       <c r="E152" s="1"/>
     </row>
     <row r="153" spans="1:5">
-      <c r="A153" s="19"/>
-      <c r="B153" s="13" t="s">
+      <c r="A153" s="24"/>
+      <c r="B153" s="14" t="s">
         <v>10</v>
       </c>
       <c r="C153" s="3" t="s">
-        <v>67</v>
+        <v>106</v>
       </c>
       <c r="D153" s="1"/>
       <c r="E153" s="1"/>
     </row>
     <row r="154" spans="1:5">
-      <c r="A154" s="19"/>
+      <c r="A154" s="24"/>
       <c r="B154" s="14" t="s">
-        <v>12</v>
+        <v>141</v>
       </c>
       <c r="C154" s="3" t="s">
-        <v>67</v>
+        <v>145</v>
       </c>
       <c r="D154" s="1"/>
       <c r="E154" s="1"/>
     </row>
     <row r="155" spans="1:5">
-      <c r="A155" s="20"/>
+      <c r="A155" s="24"/>
       <c r="B155" s="14" t="s">
-        <v>88</v>
+        <v>143</v>
       </c>
       <c r="C155" s="3" t="s">
-        <v>67</v>
+        <v>146</v>
       </c>
       <c r="D155" s="1"/>
       <c r="E155" s="1"/>
     </row>
     <row r="156" spans="1:5">
-      <c r="A156" s="21"/>
-      <c r="B156" s="22"/>
-      <c r="C156" s="22"/>
-      <c r="D156" s="22"/>
+      <c r="A156" s="23"/>
+      <c r="B156" s="23"/>
+      <c r="C156" s="23"/>
+      <c r="D156" s="23"/>
       <c r="E156" s="23"/>
     </row>
     <row r="157" spans="1:5">
       <c r="A157" s="18">
-        <v>42141</v>
+        <v>42140</v>
       </c>
       <c r="B157" s="14" t="s">
         <v>5</v>
@@ -3167,21 +3171,21 @@
       <c r="E161" s="1"/>
     </row>
     <row r="162" spans="1:5">
-      <c r="A162" s="21"/>
-      <c r="B162" s="22"/>
-      <c r="C162" s="22"/>
-      <c r="D162" s="22"/>
-      <c r="E162" s="23"/>
+      <c r="A162" s="37"/>
+      <c r="B162" s="38"/>
+      <c r="C162" s="38"/>
+      <c r="D162" s="38"/>
+      <c r="E162" s="39"/>
     </row>
     <row r="163" spans="1:5">
       <c r="A163" s="18">
-        <v>42142</v>
+        <v>42141</v>
       </c>
       <c r="B163" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C163" s="3" t="s">
-        <v>155</v>
+        <v>67</v>
       </c>
       <c r="D163" s="1"/>
       <c r="E163" s="1"/>
@@ -3192,7 +3196,7 @@
         <v>9</v>
       </c>
       <c r="C164" s="3" t="s">
-        <v>154</v>
+        <v>67</v>
       </c>
       <c r="D164" s="1"/>
       <c r="E164" s="1"/>
@@ -3203,7 +3207,7 @@
         <v>10</v>
       </c>
       <c r="C165" s="3" t="s">
-        <v>156</v>
+        <v>67</v>
       </c>
       <c r="D165" s="1"/>
       <c r="E165" s="1"/>
@@ -3214,7 +3218,7 @@
         <v>12</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>157</v>
+        <v>67</v>
       </c>
       <c r="D166" s="1"/>
       <c r="E166" s="1"/>
@@ -3225,27 +3229,27 @@
         <v>88</v>
       </c>
       <c r="C167" s="3" t="s">
-        <v>158</v>
+        <v>67</v>
       </c>
       <c r="D167" s="1"/>
       <c r="E167" s="1"/>
     </row>
     <row r="168" spans="1:5">
-      <c r="A168" s="21"/>
-      <c r="B168" s="22"/>
-      <c r="C168" s="22"/>
-      <c r="D168" s="22"/>
-      <c r="E168" s="23"/>
+      <c r="A168" s="37"/>
+      <c r="B168" s="38"/>
+      <c r="C168" s="38"/>
+      <c r="D168" s="38"/>
+      <c r="E168" s="39"/>
     </row>
     <row r="169" spans="1:5">
       <c r="A169" s="18">
-        <v>42143</v>
+        <v>42142</v>
       </c>
       <c r="B169" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="D169" s="1"/>
       <c r="E169" s="1"/>
@@ -3256,7 +3260,7 @@
         <v>9</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="D170" s="1"/>
       <c r="E170" s="1"/>
@@ -3267,7 +3271,7 @@
         <v>10</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>156</v>
+        <v>150</v>
       </c>
       <c r="D171" s="1"/>
       <c r="E171" s="1"/>
@@ -3278,7 +3282,7 @@
         <v>12</v>
       </c>
       <c r="C172" s="3" t="s">
-        <v>157</v>
+        <v>151</v>
       </c>
       <c r="D172" s="1"/>
       <c r="E172" s="1"/>
@@ -3289,27 +3293,27 @@
         <v>88</v>
       </c>
       <c r="C173" s="3" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="D173" s="1"/>
       <c r="E173" s="1"/>
     </row>
     <row r="174" spans="1:5">
-      <c r="A174" s="21"/>
-      <c r="B174" s="22"/>
-      <c r="C174" s="22"/>
-      <c r="D174" s="22"/>
-      <c r="E174" s="23"/>
+      <c r="A174" s="37"/>
+      <c r="B174" s="38"/>
+      <c r="C174" s="38"/>
+      <c r="D174" s="38"/>
+      <c r="E174" s="39"/>
     </row>
     <row r="175" spans="1:5">
       <c r="A175" s="18">
-        <v>42144</v>
+        <v>42143</v>
       </c>
       <c r="B175" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C175" s="3" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="D175" s="1"/>
       <c r="E175" s="1"/>
@@ -3320,7 +3324,7 @@
         <v>9</v>
       </c>
       <c r="C176" s="3" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="D176" s="1"/>
       <c r="E176" s="1"/>
@@ -3331,7 +3335,7 @@
         <v>10</v>
       </c>
       <c r="C177" s="3" t="s">
-        <v>162</v>
+        <v>150</v>
       </c>
       <c r="D177" s="1"/>
       <c r="E177" s="1"/>
@@ -3342,7 +3346,7 @@
         <v>12</v>
       </c>
       <c r="C178" s="3" t="s">
-        <v>163</v>
+        <v>151</v>
       </c>
       <c r="D178" s="1"/>
       <c r="E178" s="1"/>
@@ -3353,27 +3357,27 @@
         <v>88</v>
       </c>
       <c r="C179" s="3" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="D179" s="1"/>
       <c r="E179" s="1"/>
     </row>
     <row r="180" spans="1:5">
-      <c r="A180" s="21"/>
-      <c r="B180" s="22"/>
-      <c r="C180" s="22"/>
-      <c r="D180" s="22"/>
-      <c r="E180" s="23"/>
+      <c r="A180" s="37"/>
+      <c r="B180" s="38"/>
+      <c r="C180" s="38"/>
+      <c r="D180" s="38"/>
+      <c r="E180" s="39"/>
     </row>
     <row r="181" spans="1:5">
       <c r="A181" s="18">
-        <v>42145</v>
+        <v>42144</v>
       </c>
       <c r="B181" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C181" s="3" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D181" s="1"/>
       <c r="E181" s="1"/>
@@ -3384,7 +3388,7 @@
         <v>9</v>
       </c>
       <c r="C182" s="3" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
       <c r="D182" s="1"/>
       <c r="E182" s="1"/>
@@ -3395,7 +3399,7 @@
         <v>10</v>
       </c>
       <c r="C183" s="3" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D183" s="1"/>
       <c r="E183" s="1"/>
@@ -3406,7 +3410,7 @@
         <v>12</v>
       </c>
       <c r="C184" s="3" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="D184" s="1"/>
       <c r="E184" s="1"/>
@@ -3417,27 +3421,27 @@
         <v>88</v>
       </c>
       <c r="C185" s="3" t="s">
-        <v>168</v>
+        <v>158</v>
       </c>
       <c r="D185" s="1"/>
       <c r="E185" s="1"/>
     </row>
     <row r="186" spans="1:5">
-      <c r="A186" s="21"/>
-      <c r="B186" s="22"/>
-      <c r="C186" s="22"/>
-      <c r="D186" s="22"/>
-      <c r="E186" s="23"/>
+      <c r="A186" s="37"/>
+      <c r="B186" s="38"/>
+      <c r="C186" s="38"/>
+      <c r="D186" s="38"/>
+      <c r="E186" s="39"/>
     </row>
     <row r="187" spans="1:5">
       <c r="A187" s="18">
-        <v>42146</v>
+        <v>42145</v>
       </c>
       <c r="B187" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C187" s="3" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
       <c r="D187" s="1"/>
       <c r="E187" s="1"/>
@@ -3448,7 +3452,7 @@
         <v>9</v>
       </c>
       <c r="C188" s="3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D188" s="1"/>
       <c r="E188" s="1"/>
@@ -3459,7 +3463,7 @@
         <v>10</v>
       </c>
       <c r="C189" s="3" t="s">
-        <v>170</v>
+        <v>160</v>
       </c>
       <c r="D189" s="1"/>
       <c r="E189" s="1"/>
@@ -3470,7 +3474,7 @@
         <v>12</v>
       </c>
       <c r="C190" s="3" t="s">
-        <v>171</v>
+        <v>161</v>
       </c>
       <c r="D190" s="1"/>
       <c r="E190" s="1"/>
@@ -3481,27 +3485,27 @@
         <v>88</v>
       </c>
       <c r="C191" s="3" t="s">
-        <v>172</v>
+        <v>162</v>
       </c>
       <c r="D191" s="1"/>
       <c r="E191" s="1"/>
     </row>
     <row r="192" spans="1:5">
-      <c r="A192" s="21"/>
-      <c r="B192" s="22"/>
-      <c r="C192" s="22"/>
-      <c r="D192" s="22"/>
-      <c r="E192" s="23"/>
+      <c r="A192" s="37"/>
+      <c r="B192" s="38"/>
+      <c r="C192" s="38"/>
+      <c r="D192" s="38"/>
+      <c r="E192" s="39"/>
     </row>
     <row r="193" spans="1:5">
       <c r="A193" s="18">
-        <v>42147</v>
+        <v>42146</v>
       </c>
       <c r="B193" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C193" s="3" t="s">
-        <v>67</v>
+        <v>159</v>
       </c>
       <c r="D193" s="1"/>
       <c r="E193" s="1"/>
@@ -3512,7 +3516,7 @@
         <v>9</v>
       </c>
       <c r="C194" s="3" t="s">
-        <v>67</v>
+        <v>159</v>
       </c>
       <c r="D194" s="1"/>
       <c r="E194" s="1"/>
@@ -3523,7 +3527,7 @@
         <v>10</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>67</v>
+        <v>164</v>
       </c>
       <c r="D195" s="1"/>
       <c r="E195" s="1"/>
@@ -3534,7 +3538,7 @@
         <v>12</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>67</v>
+        <v>165</v>
       </c>
       <c r="D196" s="1"/>
       <c r="E196" s="1"/>
@@ -3545,21 +3549,21 @@
         <v>88</v>
       </c>
       <c r="C197" s="3" t="s">
-        <v>67</v>
+        <v>166</v>
       </c>
       <c r="D197" s="1"/>
       <c r="E197" s="1"/>
     </row>
     <row r="198" spans="1:5">
-      <c r="A198" s="21"/>
-      <c r="B198" s="22"/>
-      <c r="C198" s="22"/>
-      <c r="D198" s="22"/>
-      <c r="E198" s="23"/>
+      <c r="A198" s="37"/>
+      <c r="B198" s="38"/>
+      <c r="C198" s="38"/>
+      <c r="D198" s="38"/>
+      <c r="E198" s="39"/>
     </row>
     <row r="199" spans="1:5">
       <c r="A199" s="18">
-        <v>42148</v>
+        <v>42147</v>
       </c>
       <c r="B199" s="14" t="s">
         <v>5</v>
@@ -3615,21 +3619,21 @@
       <c r="E203" s="1"/>
     </row>
     <row r="204" spans="1:5">
-      <c r="A204" s="21"/>
-      <c r="B204" s="22"/>
-      <c r="C204" s="22"/>
-      <c r="D204" s="22"/>
-      <c r="E204" s="23"/>
+      <c r="A204" s="37"/>
+      <c r="B204" s="38"/>
+      <c r="C204" s="38"/>
+      <c r="D204" s="38"/>
+      <c r="E204" s="39"/>
     </row>
     <row r="205" spans="1:5">
       <c r="A205" s="18">
-        <v>42149</v>
+        <v>42148</v>
       </c>
       <c r="B205" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C205" s="3" t="s">
-        <v>173</v>
+        <v>67</v>
       </c>
       <c r="D205" s="1"/>
       <c r="E205" s="1"/>
@@ -3640,7 +3644,7 @@
         <v>9</v>
       </c>
       <c r="C206" s="3" t="s">
-        <v>174</v>
+        <v>67</v>
       </c>
       <c r="D206" s="1"/>
       <c r="E206" s="1"/>
@@ -3651,7 +3655,7 @@
         <v>10</v>
       </c>
       <c r="C207" s="3" t="s">
-        <v>170</v>
+        <v>67</v>
       </c>
       <c r="D207" s="1"/>
       <c r="E207" s="1"/>
@@ -3662,7 +3666,7 @@
         <v>12</v>
       </c>
       <c r="C208" s="3" t="s">
-        <v>171</v>
+        <v>67</v>
       </c>
       <c r="D208" s="1"/>
       <c r="E208" s="1"/>
@@ -3673,27 +3677,27 @@
         <v>88</v>
       </c>
       <c r="C209" s="3" t="s">
-        <v>172</v>
+        <v>67</v>
       </c>
       <c r="D209" s="1"/>
       <c r="E209" s="1"/>
     </row>
     <row r="210" spans="1:5">
-      <c r="A210" s="21"/>
-      <c r="B210" s="22"/>
-      <c r="C210" s="22"/>
-      <c r="D210" s="22"/>
-      <c r="E210" s="23"/>
+      <c r="A210" s="37"/>
+      <c r="B210" s="38"/>
+      <c r="C210" s="38"/>
+      <c r="D210" s="38"/>
+      <c r="E210" s="39"/>
     </row>
     <row r="211" spans="1:5">
       <c r="A211" s="18">
-        <v>42150</v>
+        <v>42149</v>
       </c>
       <c r="B211" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C211" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D211" s="1"/>
       <c r="E211" s="1"/>
@@ -3704,7 +3708,7 @@
         <v>9</v>
       </c>
       <c r="C212" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D212" s="1"/>
       <c r="E212" s="1"/>
@@ -3715,7 +3719,7 @@
         <v>10</v>
       </c>
       <c r="C213" s="3" t="s">
-        <v>170</v>
+        <v>164</v>
       </c>
       <c r="D213" s="1"/>
       <c r="E213" s="1"/>
@@ -3726,7 +3730,7 @@
         <v>12</v>
       </c>
       <c r="C214" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D214" s="1"/>
       <c r="E214" s="1"/>
@@ -3737,27 +3741,27 @@
         <v>88</v>
       </c>
       <c r="C215" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D215" s="1"/>
       <c r="E215" s="1"/>
     </row>
     <row r="216" spans="1:5">
-      <c r="A216" s="21"/>
-      <c r="B216" s="22"/>
-      <c r="C216" s="22"/>
-      <c r="D216" s="22"/>
-      <c r="E216" s="23"/>
+      <c r="A216" s="37"/>
+      <c r="B216" s="38"/>
+      <c r="C216" s="38"/>
+      <c r="D216" s="38"/>
+      <c r="E216" s="39"/>
     </row>
     <row r="217" spans="1:5">
       <c r="A217" s="18">
-        <v>42151</v>
+        <v>42150</v>
       </c>
       <c r="B217" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C217" s="3" t="s">
-        <v>173</v>
+        <v>167</v>
       </c>
       <c r="D217" s="1"/>
       <c r="E217" s="1"/>
@@ -3768,7 +3772,7 @@
         <v>9</v>
       </c>
       <c r="C218" s="3" t="s">
-        <v>174</v>
+        <v>168</v>
       </c>
       <c r="D218" s="1"/>
       <c r="E218" s="1"/>
@@ -3779,7 +3783,7 @@
         <v>10</v>
       </c>
       <c r="C219" s="3" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D219" s="1"/>
       <c r="E219" s="1"/>
@@ -3790,7 +3794,7 @@
         <v>12</v>
       </c>
       <c r="C220" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D220" s="1"/>
       <c r="E220" s="1"/>
@@ -3801,27 +3805,27 @@
         <v>88</v>
       </c>
       <c r="C221" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D221" s="1"/>
       <c r="E221" s="1"/>
     </row>
     <row r="222" spans="1:5">
-      <c r="A222" s="21"/>
-      <c r="B222" s="22"/>
-      <c r="C222" s="22"/>
-      <c r="D222" s="22"/>
-      <c r="E222" s="23"/>
+      <c r="A222" s="37"/>
+      <c r="B222" s="38"/>
+      <c r="C222" s="38"/>
+      <c r="D222" s="38"/>
+      <c r="E222" s="39"/>
     </row>
     <row r="223" spans="1:5">
       <c r="A223" s="18">
-        <v>42152</v>
+        <v>42151</v>
       </c>
       <c r="B223" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C223" s="3" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="D223" s="1"/>
       <c r="E223" s="1"/>
@@ -3832,7 +3836,7 @@
         <v>9</v>
       </c>
       <c r="C224" s="3" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="D224" s="1"/>
       <c r="E224" s="1"/>
@@ -3843,7 +3847,7 @@
         <v>10</v>
       </c>
       <c r="C225" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D225" s="1"/>
       <c r="E225" s="1"/>
@@ -3854,7 +3858,7 @@
         <v>12</v>
       </c>
       <c r="C226" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D226" s="1"/>
       <c r="E226" s="1"/>
@@ -3865,27 +3869,27 @@
         <v>88</v>
       </c>
       <c r="C227" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D227" s="1"/>
       <c r="E227" s="1"/>
     </row>
     <row r="228" spans="1:5">
-      <c r="A228" s="21"/>
-      <c r="B228" s="22"/>
-      <c r="C228" s="22"/>
-      <c r="D228" s="22"/>
-      <c r="E228" s="23"/>
+      <c r="A228" s="37"/>
+      <c r="B228" s="38"/>
+      <c r="C228" s="38"/>
+      <c r="D228" s="38"/>
+      <c r="E228" s="39"/>
     </row>
     <row r="229" spans="1:5">
       <c r="A229" s="18">
-        <v>42153</v>
+        <v>42152</v>
       </c>
       <c r="B229" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C229" s="3" t="s">
-        <v>176</v>
+        <v>170</v>
       </c>
       <c r="D229" s="1"/>
       <c r="E229" s="1"/>
@@ -3896,7 +3900,7 @@
         <v>9</v>
       </c>
       <c r="C230" s="3" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="D230" s="1"/>
       <c r="E230" s="1"/>
@@ -3907,7 +3911,7 @@
         <v>10</v>
       </c>
       <c r="C231" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D231" s="1"/>
       <c r="E231" s="1"/>
@@ -3918,7 +3922,7 @@
         <v>12</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D232" s="1"/>
       <c r="E232" s="1"/>
@@ -3929,27 +3933,27 @@
         <v>88</v>
       </c>
       <c r="C233" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D233" s="1"/>
       <c r="E233" s="1"/>
     </row>
     <row r="234" spans="1:5">
-      <c r="A234" s="21"/>
-      <c r="B234" s="22"/>
-      <c r="C234" s="22"/>
-      <c r="D234" s="22"/>
-      <c r="E234" s="23"/>
+      <c r="A234" s="37"/>
+      <c r="B234" s="38"/>
+      <c r="C234" s="38"/>
+      <c r="D234" s="38"/>
+      <c r="E234" s="39"/>
     </row>
     <row r="235" spans="1:5">
       <c r="A235" s="18">
-        <v>42154</v>
+        <v>42153</v>
       </c>
       <c r="B235" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C235" s="3" t="s">
-        <v>67</v>
+        <v>170</v>
       </c>
       <c r="D235" s="1"/>
       <c r="E235" s="1"/>
@@ -3960,7 +3964,7 @@
         <v>9</v>
       </c>
       <c r="C236" s="3" t="s">
-        <v>67</v>
+        <v>171</v>
       </c>
       <c r="D236" s="1"/>
       <c r="E236" s="1"/>
@@ -3971,7 +3975,7 @@
         <v>10</v>
       </c>
       <c r="C237" s="3" t="s">
-        <v>67</v>
+        <v>169</v>
       </c>
       <c r="D237" s="1"/>
       <c r="E237" s="1"/>
@@ -3982,7 +3986,7 @@
         <v>12</v>
       </c>
       <c r="C238" s="3" t="s">
-        <v>67</v>
+        <v>165</v>
       </c>
       <c r="D238" s="1"/>
       <c r="E238" s="1"/>
@@ -3993,21 +3997,21 @@
         <v>88</v>
       </c>
       <c r="C239" s="3" t="s">
-        <v>67</v>
+        <v>166</v>
       </c>
       <c r="D239" s="1"/>
       <c r="E239" s="1"/>
     </row>
     <row r="240" spans="1:5">
-      <c r="A240" s="21"/>
-      <c r="B240" s="22"/>
-      <c r="C240" s="22"/>
-      <c r="D240" s="22"/>
-      <c r="E240" s="23"/>
+      <c r="A240" s="37"/>
+      <c r="B240" s="38"/>
+      <c r="C240" s="38"/>
+      <c r="D240" s="38"/>
+      <c r="E240" s="39"/>
     </row>
     <row r="241" spans="1:5">
       <c r="A241" s="18">
-        <v>42155</v>
+        <v>42154</v>
       </c>
       <c r="B241" s="14" t="s">
         <v>5</v>
@@ -4063,21 +4067,21 @@
       <c r="E245" s="1"/>
     </row>
     <row r="246" spans="1:5">
-      <c r="A246" s="21"/>
-      <c r="B246" s="22"/>
-      <c r="C246" s="22"/>
-      <c r="D246" s="22"/>
-      <c r="E246" s="23"/>
+      <c r="A246" s="37"/>
+      <c r="B246" s="38"/>
+      <c r="C246" s="38"/>
+      <c r="D246" s="38"/>
+      <c r="E246" s="39"/>
     </row>
     <row r="247" spans="1:5">
       <c r="A247" s="18">
-        <v>42156</v>
+        <v>42155</v>
       </c>
       <c r="B247" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C247" s="3" t="s">
-        <v>178</v>
+        <v>67</v>
       </c>
       <c r="D247" s="1"/>
       <c r="E247" s="1"/>
@@ -4088,7 +4092,7 @@
         <v>9</v>
       </c>
       <c r="C248" s="3" t="s">
-        <v>179</v>
+        <v>67</v>
       </c>
       <c r="D248" s="1"/>
       <c r="E248" s="1"/>
@@ -4099,7 +4103,7 @@
         <v>10</v>
       </c>
       <c r="C249" s="3" t="s">
-        <v>175</v>
+        <v>67</v>
       </c>
       <c r="D249" s="1"/>
       <c r="E249" s="1"/>
@@ -4110,7 +4114,7 @@
         <v>12</v>
       </c>
       <c r="C250" s="3" t="s">
-        <v>171</v>
+        <v>67</v>
       </c>
       <c r="D250" s="1"/>
       <c r="E250" s="1"/>
@@ -4121,27 +4125,27 @@
         <v>88</v>
       </c>
       <c r="C251" s="3" t="s">
-        <v>172</v>
+        <v>67</v>
       </c>
       <c r="D251" s="1"/>
       <c r="E251" s="1"/>
     </row>
     <row r="252" spans="1:5">
-      <c r="A252" s="21"/>
-      <c r="B252" s="22"/>
-      <c r="C252" s="22"/>
-      <c r="D252" s="22"/>
-      <c r="E252" s="23"/>
+      <c r="A252" s="37"/>
+      <c r="B252" s="38"/>
+      <c r="C252" s="38"/>
+      <c r="D252" s="38"/>
+      <c r="E252" s="39"/>
     </row>
     <row r="253" spans="1:5">
       <c r="A253" s="18">
-        <v>42157</v>
+        <v>42156</v>
       </c>
       <c r="B253" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C253" s="3" t="s">
-        <v>178</v>
+        <v>172</v>
       </c>
       <c r="D253" s="1"/>
       <c r="E253" s="1"/>
@@ -4152,7 +4156,7 @@
         <v>9</v>
       </c>
       <c r="C254" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D254" s="1"/>
       <c r="E254" s="1"/>
@@ -4163,7 +4167,7 @@
         <v>10</v>
       </c>
       <c r="C255" s="3" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="D255" s="1"/>
       <c r="E255" s="1"/>
@@ -4174,7 +4178,7 @@
         <v>12</v>
       </c>
       <c r="C256" s="3" t="s">
-        <v>171</v>
+        <v>165</v>
       </c>
       <c r="D256" s="1"/>
       <c r="E256" s="1"/>
@@ -4185,27 +4189,27 @@
         <v>88</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>172</v>
+        <v>166</v>
       </c>
       <c r="D257" s="1"/>
       <c r="E257" s="1"/>
     </row>
     <row r="258" spans="1:5">
-      <c r="A258" s="21"/>
-      <c r="B258" s="22"/>
-      <c r="C258" s="22"/>
-      <c r="D258" s="22"/>
-      <c r="E258" s="23"/>
+      <c r="A258" s="37"/>
+      <c r="B258" s="38"/>
+      <c r="C258" s="38"/>
+      <c r="D258" s="38"/>
+      <c r="E258" s="39"/>
     </row>
     <row r="259" spans="1:5">
       <c r="A259" s="18">
-        <v>42158</v>
+        <v>42157</v>
       </c>
       <c r="B259" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C259" s="3" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="D259" s="1"/>
       <c r="E259" s="1"/>
@@ -4216,7 +4220,7 @@
         <v>9</v>
       </c>
       <c r="C260" s="3" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
       <c r="D260" s="1"/>
       <c r="E260" s="1"/>
@@ -4227,7 +4231,7 @@
         <v>10</v>
       </c>
       <c r="C261" s="3" t="s">
-        <v>181</v>
+        <v>169</v>
       </c>
       <c r="D261" s="1"/>
       <c r="E261" s="1"/>
@@ -4238,7 +4242,7 @@
         <v>12</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>182</v>
+        <v>165</v>
       </c>
       <c r="D262" s="1"/>
       <c r="E262" s="1"/>
@@ -4249,27 +4253,27 @@
         <v>88</v>
       </c>
       <c r="C263" s="3" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="D263" s="1"/>
       <c r="E263" s="1"/>
     </row>
     <row r="264" spans="1:5">
-      <c r="A264" s="21"/>
-      <c r="B264" s="22"/>
-      <c r="C264" s="22"/>
-      <c r="D264" s="22"/>
-      <c r="E264" s="23"/>
+      <c r="A264" s="37"/>
+      <c r="B264" s="38"/>
+      <c r="C264" s="38"/>
+      <c r="D264" s="38"/>
+      <c r="E264" s="39"/>
     </row>
     <row r="265" spans="1:5">
       <c r="A265" s="18">
-        <v>42159</v>
+        <v>42158</v>
       </c>
       <c r="B265" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C265" s="3" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="D265" s="1"/>
       <c r="E265" s="1"/>
@@ -4280,7 +4284,7 @@
         <v>9</v>
       </c>
       <c r="C266" s="3" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="D266" s="1"/>
       <c r="E266" s="1"/>
@@ -4291,7 +4295,7 @@
         <v>10</v>
       </c>
       <c r="C267" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D267" s="1"/>
       <c r="E267" s="1"/>
@@ -4302,7 +4306,7 @@
         <v>12</v>
       </c>
       <c r="C268" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D268" s="1"/>
       <c r="E268" s="1"/>
@@ -4313,27 +4317,27 @@
         <v>88</v>
       </c>
       <c r="C269" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D269" s="1"/>
       <c r="E269" s="1"/>
     </row>
     <row r="270" spans="1:5">
-      <c r="A270" s="21"/>
-      <c r="B270" s="22"/>
-      <c r="C270" s="22"/>
-      <c r="D270" s="22"/>
-      <c r="E270" s="23"/>
+      <c r="A270" s="37"/>
+      <c r="B270" s="38"/>
+      <c r="C270" s="38"/>
+      <c r="D270" s="38"/>
+      <c r="E270" s="39"/>
     </row>
     <row r="271" spans="1:5">
       <c r="A271" s="18">
-        <v>42160</v>
+        <v>42159</v>
       </c>
       <c r="B271" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C271" s="3" t="s">
-        <v>183</v>
+        <v>177</v>
       </c>
       <c r="D271" s="1"/>
       <c r="E271" s="1"/>
@@ -4344,7 +4348,7 @@
         <v>9</v>
       </c>
       <c r="C272" s="3" t="s">
-        <v>184</v>
+        <v>178</v>
       </c>
       <c r="D272" s="1"/>
       <c r="E272" s="1"/>
@@ -4355,7 +4359,7 @@
         <v>10</v>
       </c>
       <c r="C273" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D273" s="1"/>
       <c r="E273" s="1"/>
@@ -4366,7 +4370,7 @@
         <v>12</v>
       </c>
       <c r="C274" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D274" s="1"/>
       <c r="E274" s="1"/>
@@ -4377,27 +4381,27 @@
         <v>88</v>
       </c>
       <c r="C275" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D275" s="1"/>
       <c r="E275" s="1"/>
     </row>
     <row r="276" spans="1:5">
-      <c r="A276" s="21"/>
-      <c r="B276" s="22"/>
-      <c r="C276" s="22"/>
-      <c r="D276" s="22"/>
-      <c r="E276" s="23"/>
+      <c r="A276" s="37"/>
+      <c r="B276" s="38"/>
+      <c r="C276" s="38"/>
+      <c r="D276" s="38"/>
+      <c r="E276" s="39"/>
     </row>
     <row r="277" spans="1:5">
       <c r="A277" s="18">
-        <v>42161</v>
+        <v>42160</v>
       </c>
       <c r="B277" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C277" s="3" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="D277" s="1"/>
       <c r="E277" s="1"/>
@@ -4408,7 +4412,7 @@
         <v>9</v>
       </c>
       <c r="C278" s="3" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="D278" s="1"/>
       <c r="E278" s="1"/>
@@ -4419,7 +4423,7 @@
         <v>10</v>
       </c>
       <c r="C279" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D279" s="1"/>
       <c r="E279" s="1"/>
@@ -4430,7 +4434,7 @@
         <v>12</v>
       </c>
       <c r="C280" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D280" s="1"/>
       <c r="E280" s="1"/>
@@ -4441,27 +4445,27 @@
         <v>88</v>
       </c>
       <c r="C281" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D281" s="1"/>
       <c r="E281" s="1"/>
     </row>
     <row r="282" spans="1:5">
-      <c r="A282" s="21"/>
-      <c r="B282" s="22"/>
-      <c r="C282" s="22"/>
-      <c r="D282" s="22"/>
-      <c r="E282" s="23"/>
+      <c r="A282" s="37"/>
+      <c r="B282" s="38"/>
+      <c r="C282" s="38"/>
+      <c r="D282" s="38"/>
+      <c r="E282" s="39"/>
     </row>
     <row r="283" spans="1:5">
       <c r="A283" s="18">
-        <v>42162</v>
+        <v>42161</v>
       </c>
       <c r="B283" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C283" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D283" s="1"/>
       <c r="E283" s="1"/>
@@ -4472,7 +4476,7 @@
         <v>9</v>
       </c>
       <c r="C284" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D284" s="1"/>
       <c r="E284" s="1"/>
@@ -4483,7 +4487,7 @@
         <v>10</v>
       </c>
       <c r="C285" s="3" t="s">
-        <v>185</v>
+        <v>175</v>
       </c>
       <c r="D285" s="1"/>
       <c r="E285" s="1"/>
@@ -4494,7 +4498,7 @@
         <v>12</v>
       </c>
       <c r="C286" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D286" s="1"/>
       <c r="E286" s="1"/>
@@ -4505,27 +4509,27 @@
         <v>88</v>
       </c>
       <c r="C287" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D287" s="1"/>
       <c r="E287" s="1"/>
     </row>
     <row r="288" spans="1:5">
-      <c r="A288" s="21"/>
-      <c r="B288" s="22"/>
-      <c r="C288" s="22"/>
-      <c r="D288" s="22"/>
-      <c r="E288" s="23"/>
+      <c r="A288" s="37"/>
+      <c r="B288" s="38"/>
+      <c r="C288" s="38"/>
+      <c r="D288" s="38"/>
+      <c r="E288" s="39"/>
     </row>
     <row r="289" spans="1:5">
       <c r="A289" s="18">
-        <v>42163</v>
+        <v>42162</v>
       </c>
       <c r="B289" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C289" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D289" s="1"/>
       <c r="E289" s="1"/>
@@ -4536,7 +4540,7 @@
         <v>9</v>
       </c>
       <c r="C290" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D290" s="1"/>
       <c r="E290" s="1"/>
@@ -4547,7 +4551,7 @@
         <v>10</v>
       </c>
       <c r="C291" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D291" s="1"/>
       <c r="E291" s="1"/>
@@ -4558,7 +4562,7 @@
         <v>12</v>
       </c>
       <c r="C292" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D292" s="1"/>
       <c r="E292" s="1"/>
@@ -4569,27 +4573,27 @@
         <v>88</v>
       </c>
       <c r="C293" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D293" s="1"/>
       <c r="E293" s="1"/>
     </row>
     <row r="294" spans="1:5">
-      <c r="A294" s="21"/>
-      <c r="B294" s="22"/>
-      <c r="C294" s="22"/>
-      <c r="D294" s="22"/>
-      <c r="E294" s="23"/>
+      <c r="A294" s="37"/>
+      <c r="B294" s="38"/>
+      <c r="C294" s="38"/>
+      <c r="D294" s="38"/>
+      <c r="E294" s="39"/>
     </row>
     <row r="295" spans="1:5">
       <c r="A295" s="18">
-        <v>42164</v>
+        <v>42163</v>
       </c>
       <c r="B295" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C295" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D295" s="1"/>
       <c r="E295" s="1"/>
@@ -4600,7 +4604,7 @@
         <v>9</v>
       </c>
       <c r="C296" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D296" s="1"/>
       <c r="E296" s="1"/>
@@ -4611,7 +4615,7 @@
         <v>10</v>
       </c>
       <c r="C297" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D297" s="1"/>
       <c r="E297" s="1"/>
@@ -4622,7 +4626,7 @@
         <v>12</v>
       </c>
       <c r="C298" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D298" s="1"/>
       <c r="E298" s="1"/>
@@ -4633,27 +4637,27 @@
         <v>88</v>
       </c>
       <c r="C299" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D299" s="1"/>
       <c r="E299" s="1"/>
     </row>
     <row r="300" spans="1:5">
-      <c r="A300" s="21"/>
-      <c r="B300" s="22"/>
-      <c r="C300" s="22"/>
-      <c r="D300" s="22"/>
-      <c r="E300" s="23"/>
+      <c r="A300" s="37"/>
+      <c r="B300" s="38"/>
+      <c r="C300" s="38"/>
+      <c r="D300" s="38"/>
+      <c r="E300" s="39"/>
     </row>
     <row r="301" spans="1:5">
       <c r="A301" s="18">
-        <v>42165</v>
+        <v>42164</v>
       </c>
       <c r="B301" s="14" t="s">
         <v>5</v>
       </c>
       <c r="C301" s="3" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="D301" s="1"/>
       <c r="E301" s="1"/>
@@ -4664,7 +4668,7 @@
         <v>9</v>
       </c>
       <c r="C302" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D302" s="1"/>
       <c r="E302" s="1"/>
@@ -4675,7 +4679,7 @@
         <v>10</v>
       </c>
       <c r="C303" s="3" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="D303" s="1"/>
       <c r="E303" s="1"/>
@@ -4686,7 +4690,7 @@
         <v>12</v>
       </c>
       <c r="C304" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D304" s="1"/>
       <c r="E304" s="1"/>
@@ -4697,32 +4701,165 @@
         <v>88</v>
       </c>
       <c r="C305" s="3" t="s">
-        <v>182</v>
+        <v>176</v>
       </c>
       <c r="D305" s="1"/>
       <c r="E305" s="1"/>
     </row>
     <row r="306" spans="1:5">
-      <c r="A306" s="21"/>
-      <c r="B306" s="22"/>
-      <c r="C306" s="22"/>
-      <c r="D306" s="22"/>
-      <c r="E306" s="23"/>
+      <c r="A306" s="37"/>
+      <c r="B306" s="38"/>
+      <c r="C306" s="38"/>
+      <c r="D306" s="38"/>
+      <c r="E306" s="39"/>
+    </row>
+    <row r="307" spans="1:5">
+      <c r="A307" s="18">
+        <v>42165</v>
+      </c>
+      <c r="B307" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C307" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="D307" s="1"/>
+      <c r="E307" s="1"/>
+    </row>
+    <row r="308" spans="1:5">
+      <c r="A308" s="19"/>
+      <c r="B308" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="C308" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D308" s="1"/>
+      <c r="E308" s="1"/>
+    </row>
+    <row r="309" spans="1:5">
+      <c r="A309" s="19"/>
+      <c r="B309" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="C309" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D309" s="1"/>
+      <c r="E309" s="1"/>
+    </row>
+    <row r="310" spans="1:5">
+      <c r="A310" s="19"/>
+      <c r="B310" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C310" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D310" s="1"/>
+      <c r="E310" s="1"/>
+    </row>
+    <row r="311" spans="1:5">
+      <c r="A311" s="20"/>
+      <c r="B311" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="C311" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="D311" s="1"/>
+      <c r="E311" s="1"/>
+    </row>
+    <row r="312" spans="1:5">
+      <c r="A312" s="37"/>
+      <c r="B312" s="38"/>
+      <c r="C312" s="38"/>
+      <c r="D312" s="38"/>
+      <c r="E312" s="39"/>
     </row>
   </sheetData>
-  <mergeCells count="101">
-    <mergeCell ref="A83:A87"/>
-    <mergeCell ref="B124:B125"/>
-    <mergeCell ref="A120:A125"/>
-    <mergeCell ref="B127:B128"/>
-    <mergeCell ref="B129:B130"/>
-    <mergeCell ref="A89:A93"/>
-    <mergeCell ref="B112:B115"/>
-    <mergeCell ref="A95:A118"/>
-    <mergeCell ref="A119:E119"/>
-    <mergeCell ref="B105:B108"/>
-    <mergeCell ref="B109:B111"/>
-    <mergeCell ref="B116:B118"/>
+  <mergeCells count="103">
+    <mergeCell ref="A277:A281"/>
+    <mergeCell ref="A282:E282"/>
+    <mergeCell ref="A283:A287"/>
+    <mergeCell ref="A288:E288"/>
+    <mergeCell ref="A289:A293"/>
+    <mergeCell ref="A307:A311"/>
+    <mergeCell ref="A312:E312"/>
+    <mergeCell ref="A294:E294"/>
+    <mergeCell ref="A295:A299"/>
+    <mergeCell ref="A300:E300"/>
+    <mergeCell ref="A301:A305"/>
+    <mergeCell ref="A306:E306"/>
+    <mergeCell ref="A252:E252"/>
+    <mergeCell ref="A253:A257"/>
+    <mergeCell ref="A258:E258"/>
+    <mergeCell ref="A259:A263"/>
+    <mergeCell ref="A264:E264"/>
+    <mergeCell ref="A265:A269"/>
+    <mergeCell ref="A270:E270"/>
+    <mergeCell ref="A271:A275"/>
+    <mergeCell ref="A276:E276"/>
+    <mergeCell ref="A223:A227"/>
+    <mergeCell ref="A228:E228"/>
+    <mergeCell ref="A229:A233"/>
+    <mergeCell ref="A234:E234"/>
+    <mergeCell ref="A235:A239"/>
+    <mergeCell ref="A240:E240"/>
+    <mergeCell ref="A241:A245"/>
+    <mergeCell ref="A246:E246"/>
+    <mergeCell ref="A247:A251"/>
+    <mergeCell ref="A198:E198"/>
+    <mergeCell ref="A199:A203"/>
+    <mergeCell ref="A204:E204"/>
+    <mergeCell ref="A205:A209"/>
+    <mergeCell ref="A210:E210"/>
+    <mergeCell ref="A211:A215"/>
+    <mergeCell ref="A216:E216"/>
+    <mergeCell ref="A217:A221"/>
+    <mergeCell ref="A222:E222"/>
+    <mergeCell ref="A169:A173"/>
+    <mergeCell ref="A174:E174"/>
+    <mergeCell ref="A175:A179"/>
+    <mergeCell ref="A180:E180"/>
+    <mergeCell ref="A181:A185"/>
+    <mergeCell ref="A186:E186"/>
+    <mergeCell ref="A187:A191"/>
+    <mergeCell ref="A192:E192"/>
+    <mergeCell ref="A193:A197"/>
+    <mergeCell ref="A156:E156"/>
+    <mergeCell ref="B138:B141"/>
+    <mergeCell ref="B142:B143"/>
+    <mergeCell ref="A133:A143"/>
+    <mergeCell ref="A145:A149"/>
+    <mergeCell ref="A157:A161"/>
+    <mergeCell ref="A162:E162"/>
+    <mergeCell ref="A163:A167"/>
+    <mergeCell ref="A168:E168"/>
+    <mergeCell ref="B2:B6"/>
+    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="B13:B21"/>
+    <mergeCell ref="B24:B27"/>
+    <mergeCell ref="A13:A27"/>
+    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A151:A155"/>
+    <mergeCell ref="A132:E132"/>
+    <mergeCell ref="A144:E144"/>
+    <mergeCell ref="A150:E150"/>
+    <mergeCell ref="B122:B124"/>
+    <mergeCell ref="B125:B128"/>
+    <mergeCell ref="A28:E28"/>
+    <mergeCell ref="B29:B36"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="A29:A45"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="A46:E46"/>
+    <mergeCell ref="A82:E82"/>
+    <mergeCell ref="A88:E88"/>
+    <mergeCell ref="A47:A60"/>
+    <mergeCell ref="B59:B60"/>
     <mergeCell ref="A62:A81"/>
     <mergeCell ref="B76:B81"/>
     <mergeCell ref="B62:B69"/>
@@ -4732,86 +4869,19 @@
     <mergeCell ref="B47:B53"/>
     <mergeCell ref="B57:B58"/>
     <mergeCell ref="B95:B104"/>
-    <mergeCell ref="A28:E28"/>
-    <mergeCell ref="B29:B36"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="A29:A45"/>
-    <mergeCell ref="B44:B45"/>
-    <mergeCell ref="A46:E46"/>
-    <mergeCell ref="A82:E82"/>
-    <mergeCell ref="A88:E88"/>
     <mergeCell ref="A94:E94"/>
-    <mergeCell ref="A47:A60"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B2:B6"/>
-    <mergeCell ref="B9:B11"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="B13:B21"/>
-    <mergeCell ref="B24:B27"/>
-    <mergeCell ref="A13:A27"/>
-    <mergeCell ref="A12:E12"/>
-    <mergeCell ref="A145:A149"/>
-    <mergeCell ref="A126:E126"/>
-    <mergeCell ref="A138:E138"/>
-    <mergeCell ref="A144:E144"/>
-    <mergeCell ref="A150:E150"/>
-    <mergeCell ref="B132:B135"/>
-    <mergeCell ref="B136:B137"/>
-    <mergeCell ref="A127:A137"/>
-    <mergeCell ref="A139:A143"/>
-    <mergeCell ref="A151:A155"/>
-    <mergeCell ref="A156:E156"/>
-    <mergeCell ref="A157:A161"/>
-    <mergeCell ref="A162:E162"/>
-    <mergeCell ref="A163:A167"/>
-    <mergeCell ref="A168:E168"/>
-    <mergeCell ref="A169:A173"/>
-    <mergeCell ref="A174:E174"/>
-    <mergeCell ref="A175:A179"/>
-    <mergeCell ref="A180:E180"/>
-    <mergeCell ref="A181:A185"/>
-    <mergeCell ref="A186:E186"/>
-    <mergeCell ref="A187:A191"/>
-    <mergeCell ref="A192:E192"/>
-    <mergeCell ref="A193:A197"/>
-    <mergeCell ref="A198:E198"/>
-    <mergeCell ref="A199:A203"/>
-    <mergeCell ref="A204:E204"/>
-    <mergeCell ref="A205:A209"/>
-    <mergeCell ref="A210:E210"/>
-    <mergeCell ref="A211:A215"/>
-    <mergeCell ref="A216:E216"/>
-    <mergeCell ref="A217:A221"/>
-    <mergeCell ref="A222:E222"/>
-    <mergeCell ref="A223:A227"/>
-    <mergeCell ref="A228:E228"/>
-    <mergeCell ref="A229:A233"/>
-    <mergeCell ref="A234:E234"/>
-    <mergeCell ref="A235:A239"/>
-    <mergeCell ref="A240:E240"/>
-    <mergeCell ref="A241:A245"/>
-    <mergeCell ref="A246:E246"/>
-    <mergeCell ref="A247:A251"/>
-    <mergeCell ref="A252:E252"/>
-    <mergeCell ref="A253:A257"/>
-    <mergeCell ref="A258:E258"/>
-    <mergeCell ref="A259:A263"/>
-    <mergeCell ref="A264:E264"/>
-    <mergeCell ref="A265:A269"/>
-    <mergeCell ref="A270:E270"/>
-    <mergeCell ref="A271:A275"/>
-    <mergeCell ref="A276:E276"/>
-    <mergeCell ref="A277:A281"/>
-    <mergeCell ref="A282:E282"/>
-    <mergeCell ref="A283:A287"/>
-    <mergeCell ref="A301:A305"/>
-    <mergeCell ref="A306:E306"/>
-    <mergeCell ref="A288:E288"/>
-    <mergeCell ref="A289:A293"/>
-    <mergeCell ref="A294:E294"/>
-    <mergeCell ref="A295:A299"/>
-    <mergeCell ref="A300:E300"/>
+    <mergeCell ref="A83:A87"/>
+    <mergeCell ref="B129:B131"/>
+    <mergeCell ref="A120:A131"/>
+    <mergeCell ref="B133:B134"/>
+    <mergeCell ref="B135:B136"/>
+    <mergeCell ref="A89:A93"/>
+    <mergeCell ref="B112:B115"/>
+    <mergeCell ref="A95:A118"/>
+    <mergeCell ref="A119:E119"/>
+    <mergeCell ref="B105:B108"/>
+    <mergeCell ref="B109:B111"/>
+    <mergeCell ref="B116:B118"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>